<commit_message>
novas analises e decisão para inicio de documentação do projeto
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7050" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="principal" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>vhfaz</author>
+  </authors>
+  <commentList>
+    <comment ref="H46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Arial"/>
+            <charset val="0"/>
+          </rPr>
+          <t>vhfaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Arial"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Por conta deste resultado o processo de segmentação de grupos será de forma empirica
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Imagem</t>
   </si>
@@ -208,19 +241,50 @@
   </si>
   <si>
     <t>3 Grupos</t>
+  </si>
+  <si>
+    <t>Empirico</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Variancia</t>
+  </si>
+  <si>
+    <t>Desvio Padrão</t>
+  </si>
+  <si>
+    <t>Buscar outras</t>
+  </si>
+  <si>
+    <t>Raiz Quadrada da quantidade de valores</t>
+  </si>
+  <si>
+    <t>Quantidade de Grupos</t>
+  </si>
+  <si>
+    <t>Inicial</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,8 +468,19 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,20 +495,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.6"/>
         <bgColor rgb="FF0000F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFAFC00"/>
         <bgColor rgb="FFFAFC00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FE00"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FF00FE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -795,7 +900,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
@@ -819,16 +924,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="8">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9">
@@ -837,89 +942,89 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="35" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="37" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="40" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="41" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="43" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -933,11 +1038,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1304,35 +1415,35 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="43.5809523809524" customWidth="1"/>
-    <col min="2" max="2" width="21.7238095238095" style="14" customWidth="1"/>
-    <col min="3" max="3" width="24.7238095238095" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.8666666666667" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.0095238095238" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.7238095238095" style="20" customWidth="1"/>
+    <col min="3" max="3" width="24.7238095238095" style="21" customWidth="1"/>
+    <col min="4" max="4" width="14.8666666666667" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.0095238095238" style="21" customWidth="1"/>
     <col min="6" max="7" width="13.5809523809524" customWidth="1"/>
-    <col min="8" max="8" width="8.58095238095238" style="16" customWidth="1"/>
+    <col min="8" max="8" width="8.58095238095238" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1340,16 +1451,16 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="23">
         <v>63</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="24">
         <v>95.2380952380952</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="24">
         <v>2.48294005070334</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="24">
         <v>32095.8253968254</v>
       </c>
     </row>
@@ -1357,16 +1468,16 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="23">
         <v>143</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="24">
         <v>88.1118881118881</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="24">
         <v>1.364444446432</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="24">
         <v>11173.8624708625</v>
       </c>
     </row>
@@ -1374,16 +1485,16 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="23">
         <v>144</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="24">
         <v>96.5277777777778</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="24">
         <v>1.70932843725875</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="24">
         <v>22821.5324074074</v>
       </c>
     </row>
@@ -1391,16 +1502,16 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="23">
         <v>169</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="24">
         <v>89.9408284023669</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="24">
         <v>1.48333816024989</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="24">
         <v>17320.8165680473</v>
       </c>
     </row>
@@ -1408,16 +1519,16 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="23">
         <v>192</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="24">
         <v>88.5416666666667</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="24">
         <v>0.839565155117189</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="24">
         <v>7835.71527777778</v>
       </c>
     </row>
@@ -1425,16 +1536,16 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="23">
         <v>195</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="24">
         <v>92.3076923076923</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="24">
         <v>1.57529946585297</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="24">
         <v>20234.0512820513</v>
       </c>
     </row>
@@ -1442,16 +1553,16 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="23">
         <v>342</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="24">
         <v>78.6549707602339</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="24">
         <v>2.54102522240269</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="24">
         <v>21623.4385964912</v>
       </c>
     </row>
@@ -1459,16 +1570,16 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="23">
         <v>360</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="24">
         <v>90.2777777777778</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="24">
         <v>0.83530604292899</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="24">
         <v>15975.3722222222</v>
       </c>
     </row>
@@ -1476,16 +1587,16 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="23">
         <v>567</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="24">
         <v>83.0687830687831</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="24">
         <v>0.764069959883054</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="24">
         <v>8302.47971781305</v>
       </c>
     </row>
@@ -1493,16 +1604,16 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="23">
         <v>957</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="24">
         <v>78.7878787878788</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="24">
         <v>1.20010193064723</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="24">
         <v>11768.3869731801</v>
       </c>
     </row>
@@ -1510,16 +1621,16 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="23">
         <v>960</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="24">
         <v>80.7291666666667</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="24">
         <v>1.37105877857771</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="24">
         <v>12348.5236111111</v>
       </c>
     </row>
@@ -1527,16 +1638,16 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C13" s="18">
+      <c r="B13" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C13" s="24">
         <v>51.85546875</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="24">
         <v>0.838312805519442</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="24">
         <v>12540.5504557292</v>
       </c>
     </row>
@@ -1544,16 +1655,16 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C14" s="18">
+      <c r="B14" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C14" s="24">
         <v>60.15625</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="24">
         <v>0.845898875200358</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="24">
         <v>5979.56608072917</v>
       </c>
     </row>
@@ -1561,16 +1672,16 @@
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C15" s="18">
+      <c r="B15" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C15" s="24">
         <v>69.23828125</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="24">
         <v>0.797975851545744</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="24">
         <v>13772.6712239583</v>
       </c>
     </row>
@@ -1578,16 +1689,16 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C16" s="18">
+      <c r="B16" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C16" s="24">
         <v>71.97265625</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="24">
         <v>0.90723544826971</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="24">
         <v>6634.69661458333</v>
       </c>
     </row>
@@ -1595,16 +1706,16 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C17" s="18">
+      <c r="B17" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C17" s="24">
         <v>82.91015625</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="24">
         <v>1.08457882938325</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="24">
         <v>7699.07421875</v>
       </c>
     </row>
@@ -1612,16 +1723,16 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C18" s="18">
+      <c r="B18" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C18" s="24">
         <v>84.86328125</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="24">
         <v>0.922550790721476</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="24">
         <v>8025.58561197917</v>
       </c>
     </row>
@@ -1629,16 +1740,16 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C19" s="18">
+      <c r="B19" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C19" s="24">
         <v>89.84375</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="24">
         <v>1.0160852567902</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="24">
         <v>8118.27180989583</v>
       </c>
     </row>
@@ -1646,16 +1757,16 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C20" s="18">
+      <c r="B20" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C20" s="24">
         <v>90.625</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="24">
         <v>1.07335028417615</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="24">
         <v>9339.25813802083</v>
       </c>
     </row>
@@ -1663,16 +1774,16 @@
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C21" s="18">
+      <c r="B21" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C21" s="24">
         <v>91.30859375</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="24">
         <v>0.693335440701425</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="24">
         <v>9839.32259114583</v>
       </c>
     </row>
@@ -1680,16 +1791,16 @@
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C22" s="18">
+      <c r="B22" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C22" s="24">
         <v>93.45703125</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="24">
         <v>0.806533165989523</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="24">
         <v>7061.1376953125</v>
       </c>
     </row>
@@ -1697,16 +1808,16 @@
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C23" s="18">
+      <c r="B23" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C23" s="24">
         <v>94.04296875</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="24">
         <v>1.14457765338719</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="24">
         <v>6324.42740885417</v>
       </c>
     </row>
@@ -1714,19 +1825,19 @@
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C24" s="18">
+      <c r="B24" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C24" s="24">
         <v>94.43359375</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="24">
         <v>1.02464606740115</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="24">
         <v>5216.81217447917</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="25">
         <f>QUARTILE(B2:B51,1)</f>
         <v>1024</v>
       </c>
@@ -1735,19 +1846,19 @@
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C25" s="18">
+      <c r="B25" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C25" s="24">
         <v>95.41015625</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="24">
         <v>0.789110995517099</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="24">
         <v>6441.08235677083</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="24">
         <f>QUARTILE(B2:B51,3)</f>
         <v>1820.25</v>
       </c>
@@ -1756,19 +1867,19 @@
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C26" s="18">
+      <c r="B26" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C26" s="24">
         <v>96.484375</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="24">
         <v>1.18278038952791</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="24">
         <v>5653.32389322917</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="24">
         <f>H25-H24</f>
         <v>796.25</v>
       </c>
@@ -1777,16 +1888,16 @@
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C27" s="18">
+      <c r="B27" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C27" s="24">
         <v>96.6796875</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="24">
         <v>0.924962425624733</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="24">
         <v>9505.28971354167</v>
       </c>
     </row>
@@ -1794,16 +1905,16 @@
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C28" s="18">
+      <c r="B28" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C28" s="24">
         <v>97.55859375</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="24">
         <v>0.779331859488869</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="24">
         <v>6480.76627604167</v>
       </c>
     </row>
@@ -1811,16 +1922,16 @@
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C29" s="18">
+      <c r="B29" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C29" s="24">
         <v>97.75390625</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="24">
         <v>1.03331199141793</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="24">
         <v>7881.16015625</v>
       </c>
     </row>
@@ -1828,16 +1939,16 @@
       <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C30" s="18">
+      <c r="B30" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C30" s="24">
         <v>98.33984375</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="24">
         <v>1.03331808024201</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="24">
         <v>5696.2646484375</v>
       </c>
     </row>
@@ -1845,16 +1956,16 @@
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C31" s="18">
+      <c r="B31" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C31" s="24">
         <v>98.828125</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="24">
         <v>0.820182535969992</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="24">
         <v>7171.57552083333</v>
       </c>
     </row>
@@ -1862,16 +1973,16 @@
       <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C32" s="18">
+      <c r="B32" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C32" s="24">
         <v>98.92578125</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="24">
         <v>1.66662067220565</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="24">
         <v>5223.94759114583</v>
       </c>
     </row>
@@ -1879,16 +1990,16 @@
       <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C33" s="18">
+      <c r="B33" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C33" s="24">
         <v>99.0234375</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="24">
         <v>1.02693685083336</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="24">
         <v>7127.9765625</v>
       </c>
     </row>
@@ -1896,16 +2007,16 @@
       <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C34" s="18">
+      <c r="B34" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C34" s="24">
         <v>99.31640625</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34" s="24">
         <v>0.789110502896811</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="24">
         <v>7219.12044270833</v>
       </c>
     </row>
@@ -1913,16 +2024,16 @@
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C35" s="18">
+      <c r="B35" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C35" s="24">
         <v>99.90234375</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="24">
         <v>1.33843056044939</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="24">
         <v>5544.04752604167</v>
       </c>
     </row>
@@ -1930,16 +2041,16 @@
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="17">
-        <v>1024</v>
-      </c>
-      <c r="C36" s="19">
+      <c r="B36" s="23">
+        <v>1024</v>
+      </c>
+      <c r="C36" s="25">
         <v>100</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="24">
         <v>0.782071413305328</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="24">
         <v>4360.73274739583</v>
       </c>
     </row>
@@ -1947,16 +2058,16 @@
       <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="23">
         <v>1485</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="24">
         <v>92.6599326599327</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D37" s="24">
         <v>1.32274471267522</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="24">
         <v>14957.0799102132</v>
       </c>
     </row>
@@ -1964,16 +2075,16 @@
       <c r="A38" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="23">
         <v>1485</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="24">
         <v>96.2962962962963</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D38" s="24">
         <v>1.45405057678211</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="24">
         <v>16642.0053872054</v>
       </c>
     </row>
@@ -1981,16 +2092,16 @@
       <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="23">
         <v>1932</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="24">
         <v>87.9399585921325</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="24">
         <v>3.67039288099722</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="24">
         <v>13846.0163906142</v>
       </c>
     </row>
@@ -1998,16 +2109,16 @@
       <c r="A40" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="23">
         <v>2048</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="24">
         <v>97.900390625</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D40" s="24">
         <v>1.06513926941072</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="24">
         <v>52975.3678385417</v>
       </c>
     </row>
@@ -2015,16 +2126,16 @@
       <c r="A41" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="23">
         <v>2268</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="24">
         <v>67.636684303351</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D41" s="24">
         <v>2.78715706602952</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="24">
         <v>9633.48633156967</v>
       </c>
     </row>
@@ -2032,16 +2143,16 @@
       <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="23">
         <v>6400</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="24">
         <v>62.1875</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="24">
         <v>1.03810485467137</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="24">
         <v>52610.26671875</v>
       </c>
     </row>
@@ -2049,16 +2160,16 @@
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="23">
         <v>7168</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="24">
         <v>45.1729910714286</v>
       </c>
-      <c r="D43" s="18">
+      <c r="D43" s="24">
         <v>0.943255902999851</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="24">
         <v>47277.6180710566</v>
       </c>
     </row>
@@ -2066,16 +2177,16 @@
       <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="23">
         <v>7371</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="24">
         <v>90.7610907610908</v>
       </c>
-      <c r="D44" s="18">
+      <c r="D44" s="24">
         <v>2.11932991686787</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="24">
         <v>9465.43544521322</v>
       </c>
     </row>
@@ -2083,16 +2194,16 @@
       <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="23">
         <v>8960</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="24">
         <v>92.9464285714286</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="24">
         <v>1.04107091626619</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="24">
         <v>55419.8899553571</v>
       </c>
     </row>
@@ -2100,16 +2211,16 @@
       <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="23">
         <v>8960</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="24">
         <v>92.96875</v>
       </c>
-      <c r="D46" s="18">
+      <c r="D46" s="24">
         <v>1.0601274830389</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="24">
         <v>57465.4501488095</v>
       </c>
     </row>
@@ -2117,16 +2228,16 @@
       <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="17">
+      <c r="B47" s="23">
         <v>10752</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="24">
         <v>94.3452380952381</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D47" s="24">
         <v>1.00784041032555</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="24">
         <v>62213.2716393849</v>
       </c>
     </row>
@@ -2134,16 +2245,16 @@
       <c r="A48" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B48" s="23">
         <v>13625</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C48" s="24">
         <v>89.6880733944954</v>
       </c>
-      <c r="D48" s="18">
+      <c r="D48" s="24">
         <v>1.2478457181313</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48" s="24">
         <v>7128.51464220184</v>
       </c>
     </row>
@@ -2151,16 +2262,16 @@
       <c r="A49" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="23">
         <v>16616</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="24">
         <v>73.4954260953298</v>
       </c>
-      <c r="D49" s="18">
+      <c r="D49" s="24">
         <v>3.27027215449622</v>
       </c>
-      <c r="E49" s="18">
+      <c r="E49" s="24">
         <v>12746.4247512438</v>
       </c>
     </row>
@@ -2168,16 +2279,16 @@
       <c r="A50" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="17">
+      <c r="B50" s="23">
         <v>45056</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="24">
         <v>62.2181285511364</v>
       </c>
-      <c r="D50" s="18">
+      <c r="D50" s="24">
         <v>1.43638628256647</v>
       </c>
-      <c r="E50" s="18">
+      <c r="E50" s="24">
         <v>18146.4140107126</v>
       </c>
     </row>
@@ -2185,16 +2296,16 @@
       <c r="A51" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="17">
+      <c r="B51" s="23">
         <v>45056</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="24">
         <v>70.8473899147727</v>
       </c>
-      <c r="D51" s="18">
+      <c r="D51" s="24">
         <v>1.30926504569214</v>
       </c>
-      <c r="E51" s="18">
+      <c r="E51" s="24">
         <v>13996.7092581084</v>
       </c>
     </row>
@@ -2209,15 +2320,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:XFD52"/>
+  <dimension ref="A1:XFD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="9.28571428571429" customWidth="1"/>
+    <col min="7" max="7" width="40.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="9.57142857142857"/>
+    <col min="9" max="9" width="14"/>
+    <col min="10" max="10" width="13.2952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:1">
@@ -2225,7 +2340,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" spans="1:4">
+    <row r="2" ht="18.75" customHeight="1" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -2235,11 +2350,26 @@
       <c r="C2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="5">
         <v>63</v>
       </c>
@@ -2252,8 +2382,11 @@
       <c r="D3" s="6">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="5">
         <v>143</v>
       </c>
@@ -2266,8 +2399,11 @@
       <c r="D4" s="6">
         <v>143</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="5">
         <v>144</v>
       </c>
@@ -2280,8 +2416,11 @@
       <c r="D5" s="6">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="5">
         <v>169</v>
       </c>
@@ -2294,8 +2433,11 @@
       <c r="D6" s="6">
         <v>169</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="5">
         <v>192</v>
       </c>
@@ -2308,8 +2450,11 @@
       <c r="D7" s="6">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="7">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="5">
         <v>195</v>
       </c>
@@ -2322,8 +2467,11 @@
       <c r="D8" s="6">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="7">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
         <v>342</v>
       </c>
@@ -2336,8 +2484,11 @@
       <c r="D9" s="6">
         <v>342</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="7">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
         <v>360</v>
       </c>
@@ -2350,8 +2501,11 @@
       <c r="D10" s="6">
         <v>360</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="5">
         <v>567</v>
       </c>
@@ -2364,9 +2518,12 @@
       <c r="D11" s="6">
         <v>567</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7">
+      <c r="E11" s="7">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="8">
         <v>957</v>
       </c>
       <c r="B12" s="5">
@@ -2378,9 +2535,12 @@
       <c r="D12" s="6">
         <v>957</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7">
+      <c r="E12" s="7">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="8">
         <v>960</v>
       </c>
       <c r="B13" s="5">
@@ -2392,9 +2552,12 @@
       <c r="D13" s="6">
         <v>960</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7">
+      <c r="E13" s="7">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="8">
         <v>1024</v>
       </c>
       <c r="B14" s="5">
@@ -2406,9 +2569,12 @@
       <c r="D14" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7">
+      <c r="E14" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="8">
         <v>1024</v>
       </c>
       <c r="B15" s="5">
@@ -2420,9 +2586,12 @@
       <c r="D15" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7">
+      <c r="E15" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="8">
         <v>1024</v>
       </c>
       <c r="B16" s="5">
@@ -2434,9 +2603,12 @@
       <c r="D16" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7">
+      <c r="E16" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8">
         <v>1024</v>
       </c>
       <c r="B17" s="5">
@@ -2448,9 +2620,12 @@
       <c r="D17" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7">
+      <c r="E17" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8">
         <v>1024</v>
       </c>
       <c r="B18" s="5">
@@ -2462,9 +2637,12 @@
       <c r="D18" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7">
+      <c r="E18" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="8">
         <v>1024</v>
       </c>
       <c r="B19" s="5">
@@ -2476,9 +2654,12 @@
       <c r="D19" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7">
+      <c r="E19" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="8">
         <v>1024</v>
       </c>
       <c r="B20" s="5">
@@ -2490,9 +2671,12 @@
       <c r="D20" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="7">
+      <c r="E20" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8">
         <v>1024</v>
       </c>
       <c r="B21" s="5">
@@ -2504,9 +2688,12 @@
       <c r="D21" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7">
+      <c r="E21" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="8">
         <v>1024</v>
       </c>
       <c r="B22" s="5">
@@ -2518,9 +2705,12 @@
       <c r="D22" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7">
+      <c r="E22" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="8">
         <v>1024</v>
       </c>
       <c r="B23" s="5">
@@ -2532,9 +2722,12 @@
       <c r="D23" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7">
+      <c r="E23" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8">
         <v>1024</v>
       </c>
       <c r="B24" s="5">
@@ -2546,9 +2739,12 @@
       <c r="D24" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="7">
+      <c r="E24" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8">
         <v>1024</v>
       </c>
       <c r="B25" s="5">
@@ -2560,9 +2756,12 @@
       <c r="D25" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="7">
+      <c r="E25" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8">
         <v>1024</v>
       </c>
       <c r="B26" s="5">
@@ -2574,9 +2773,12 @@
       <c r="D26" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7">
+      <c r="E26" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8">
         <v>1024</v>
       </c>
       <c r="B27" s="5">
@@ -2588,9 +2790,12 @@
       <c r="D27" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="7">
+      <c r="E27" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="8">
         <v>1024</v>
       </c>
       <c r="B28" s="5">
@@ -2602,9 +2807,12 @@
       <c r="D28" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="7">
+      <c r="E28" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8">
         <v>1024</v>
       </c>
       <c r="B29" s="5">
@@ -2616,9 +2824,12 @@
       <c r="D29" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7">
+      <c r="E29" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="8">
         <v>1024</v>
       </c>
       <c r="B30" s="5">
@@ -2630,9 +2841,12 @@
       <c r="D30" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="7">
+      <c r="E30" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="8">
         <v>1024</v>
       </c>
       <c r="B31" s="5">
@@ -2644,9 +2858,12 @@
       <c r="D31" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="7">
+      <c r="E31" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8">
         <v>1024</v>
       </c>
       <c r="B32" s="5">
@@ -2658,9 +2875,12 @@
       <c r="D32" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="7">
+      <c r="E32" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="8">
         <v>1024</v>
       </c>
       <c r="B33" s="5">
@@ -2672,9 +2892,12 @@
       <c r="D33" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="7">
+      <c r="E33" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="8">
         <v>1024</v>
       </c>
       <c r="B34" s="5">
@@ -2686,9 +2909,12 @@
       <c r="D34" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="7">
+      <c r="E34" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="8">
         <v>1024</v>
       </c>
       <c r="B35" s="5">
@@ -2700,9 +2926,12 @@
       <c r="D35" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="7">
+      <c r="E35" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="8">
         <v>1024</v>
       </c>
       <c r="B36" s="5">
@@ -2714,9 +2943,12 @@
       <c r="D36" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="7">
+      <c r="E36" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="8">
         <v>1024</v>
       </c>
       <c r="B37" s="5">
@@ -2728,9 +2960,12 @@
       <c r="D37" s="6">
         <v>1024</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="7">
+      <c r="E37" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="8">
         <v>1485</v>
       </c>
       <c r="B38" s="5">
@@ -2742,9 +2977,12 @@
       <c r="D38" s="6">
         <v>1485</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="7">
+      <c r="E38" s="9">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="8">
         <v>1485</v>
       </c>
       <c r="B39" s="5">
@@ -2756,9 +2994,12 @@
       <c r="D39" s="6">
         <v>1485</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="7">
+      <c r="E39" s="9">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="8">
         <v>1932</v>
       </c>
       <c r="B40" s="5">
@@ -2770,9 +3011,12 @@
       <c r="D40" s="6">
         <v>1932</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="7">
+      <c r="E40" s="9">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="8">
         <v>2048</v>
       </c>
       <c r="B41" s="5">
@@ -2784,9 +3028,12 @@
       <c r="D41" s="6">
         <v>2048</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="7">
+      <c r="E41" s="9">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="8">
         <v>2268</v>
       </c>
       <c r="B42" s="5">
@@ -2798,145 +3045,294 @@
       <c r="D42" s="6">
         <v>2268</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="8">
+      <c r="E42" s="9">
+        <v>2268</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="11">
         <v>6400</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="8">
         <v>6400</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="8">
         <v>6400</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="8">
         <v>6400</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="8">
+      <c r="E43" s="12">
+        <v>6400</v>
+      </c>
+      <c r="G43" s="10">
+        <f>SQRT(COUNT(A3:A52))</f>
+        <v>7.07106781186548</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="11">
         <v>7168</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="8">
         <v>7168</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="8">
         <v>7168</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="8">
         <v>7168</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="8">
+      <c r="E44" s="12">
+        <v>7168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="11">
         <v>7371</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="8">
         <v>7371</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="8">
         <v>7371</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="8">
         <v>7371</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="10">
+      <c r="E45" s="12">
+        <v>7371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="13">
         <v>8960</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="11">
         <v>8960</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="8">
         <v>8960</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="8">
         <v>8960</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="10">
+      <c r="E46" s="12">
         <v>8960</v>
       </c>
-      <c r="B47" s="8">
+      <c r="G46" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="13">
         <v>8960</v>
       </c>
-      <c r="C47" s="7">
+      <c r="B47" s="11">
         <v>8960</v>
       </c>
-      <c r="D47" s="9">
+      <c r="C47" s="8">
         <v>8960</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="10">
+      <c r="D47" s="8">
+        <v>8960</v>
+      </c>
+      <c r="E47" s="12">
+        <v>8960</v>
+      </c>
+      <c r="G47" s="10">
+        <v>7</v>
+      </c>
+      <c r="H47" s="10">
+        <f>E3</f>
+        <v>63</v>
+      </c>
+      <c r="I47" s="15">
+        <f>H47+$G$49</f>
+        <v>6490.57142857143</v>
+      </c>
+      <c r="J47" s="10">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I47)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="13">
         <v>10752</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="11">
         <v>10752</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="8">
         <v>10752</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="8">
         <v>10752</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="11">
+      <c r="E48" s="14">
+        <v>10752</v>
+      </c>
+      <c r="G48">
+        <f>A52-A3</f>
+        <v>44993</v>
+      </c>
+      <c r="H48" s="15">
+        <f>I47</f>
+        <v>6490.57142857143</v>
+      </c>
+      <c r="I48" s="15">
+        <f>H48+$G$49</f>
+        <v>12918.1428571429</v>
+      </c>
+      <c r="J48" s="10">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I48)-J47</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="16">
         <v>13625</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="13">
         <v>13625</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="11">
         <v>13625</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="8">
         <v>13625</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="11">
+      <c r="E49" s="14">
+        <v>13625</v>
+      </c>
+      <c r="G49">
+        <f>G48/G47</f>
+        <v>6427.57142857143</v>
+      </c>
+      <c r="H49" s="15">
+        <f>I48</f>
+        <v>12918.1428571429</v>
+      </c>
+      <c r="I49" s="15">
+        <f>H49+$G$49</f>
+        <v>19345.7142857143</v>
+      </c>
+      <c r="J49" s="15">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I49)-SUM(J47:J48)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="16">
         <v>16616</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="13">
         <v>16616</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="11">
         <v>16616</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="8">
         <v>16616</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="12">
+      <c r="E50" s="14">
+        <v>16616</v>
+      </c>
+      <c r="H50" s="15">
+        <f>I49</f>
+        <v>19345.7142857143</v>
+      </c>
+      <c r="I50" s="15">
+        <f>H50+$G$49</f>
+        <v>25773.2857142857</v>
+      </c>
+      <c r="J50" s="15">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I50)-SUM(J47:J49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="17">
         <v>45056</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="16">
         <v>45056</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="13">
         <v>45056</v>
       </c>
-      <c r="D51" s="13">
+      <c r="D51" s="18">
         <v>45056</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="12">
+      <c r="E51" s="19">
         <v>45056</v>
       </c>
-      <c r="B52" s="11">
+      <c r="H51" s="15">
+        <f>I50</f>
+        <v>25773.2857142857</v>
+      </c>
+      <c r="I51" s="15">
+        <f>H51+$G$49</f>
+        <v>32200.8571428571</v>
+      </c>
+      <c r="J51" s="15">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I51)-SUM(J47:J50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="17">
         <v>45056</v>
       </c>
-      <c r="C52" s="10">
+      <c r="B52" s="16">
         <v>45056</v>
       </c>
-      <c r="D52" s="13">
+      <c r="C52" s="13">
         <v>45056</v>
+      </c>
+      <c r="D52" s="18">
+        <v>45056</v>
+      </c>
+      <c r="E52" s="19">
+        <v>45056</v>
+      </c>
+      <c r="H52" s="15">
+        <f>I51</f>
+        <v>32200.8571428571</v>
+      </c>
+      <c r="I52" s="15">
+        <f>H52+$G$49</f>
+        <v>38628.4285714286</v>
+      </c>
+      <c r="J52" s="15">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I52)-SUM(J47:J51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="8:10">
+      <c r="H53" s="15">
+        <f>I52</f>
+        <v>38628.4285714286</v>
+      </c>
+      <c r="I53" s="15">
+        <f>H53+$G$49</f>
+        <v>45056</v>
+      </c>
+      <c r="J53" s="15">
+        <f>COUNTIF($E$3:$E$52,"&lt;"&amp;I53)-SUM(J47:J52)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2945,5 +3341,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dados gerados com sucesso
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -7,9 +7,9 @@
     <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="dados" sheetId="3" r:id="rId1"/>
-    <sheet name="principal" sheetId="1" r:id="rId2"/>
-    <sheet name="analise" sheetId="2" r:id="rId3"/>
+    <sheet name="dados" sheetId="1" r:id="rId1"/>
+    <sheet name="principal" sheetId="2" r:id="rId2"/>
+    <sheet name="analise" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
   <si>
     <t>Imagem</t>
   </si>
@@ -70,154 +70,154 @@
     <t>Erro quadrático</t>
   </si>
   <si>
+    <t>01_dish.png</t>
+  </si>
+  <si>
+    <t>05_apple_pie.png</t>
+  </si>
+  <si>
+    <t>07_bread.png</t>
+  </si>
+  <si>
+    <t>09_baguette.png</t>
+  </si>
+  <si>
+    <t>11_bun.png</t>
+  </si>
+  <si>
+    <t>13_bacon.png</t>
+  </si>
+  <si>
+    <t>15_burger.png</t>
+  </si>
+  <si>
+    <t>18_burrito.png</t>
+  </si>
+  <si>
+    <t>20_bagel.png</t>
+  </si>
+  <si>
+    <t>22_cheesecake.png</t>
+  </si>
+  <si>
+    <t>24_cheesepuff.png</t>
+  </si>
+  <si>
+    <t>26_chocolate.png</t>
+  </si>
+  <si>
+    <t>28_cookies.png</t>
+  </si>
+  <si>
+    <t>30_chocolatecake.png</t>
+  </si>
+  <si>
+    <t>32_curry.png</t>
+  </si>
+  <si>
+    <t>34_donut.png</t>
+  </si>
+  <si>
+    <t>35_donut_dish.png</t>
+  </si>
+  <si>
+    <t>36_dumplings.png</t>
+  </si>
+  <si>
+    <t>38_friedegg.png</t>
+  </si>
+  <si>
+    <t>40_eggsalad.png</t>
+  </si>
+  <si>
+    <t>41_eggsalad_bowl.png</t>
+  </si>
+  <si>
+    <t>42_eggtart.png</t>
+  </si>
+  <si>
+    <t>44_frenchfries.png</t>
+  </si>
+  <si>
+    <t>99_taco.png</t>
+  </si>
+  <si>
+    <t>Assault-Class.png</t>
+  </si>
+  <si>
+    <t>Base.png</t>
+  </si>
+  <si>
+    <t>Basic Humanoid Sprites 1x.png</t>
+  </si>
+  <si>
+    <t>clouds.png</t>
+  </si>
+  <si>
+    <t>CuriousMonkeyIdleSide.png</t>
+  </si>
+  <si>
+    <t>demon-idle.png</t>
+  </si>
+  <si>
+    <t>example_128x128.png</t>
+  </si>
+  <si>
+    <t>example_16x16.png</t>
+  </si>
+  <si>
+    <t>example_21x27.png</t>
+  </si>
+  <si>
+    <t>Free Sprites 1x.png</t>
+  </si>
+  <si>
+    <t>ghost-shriek.png</t>
+  </si>
+  <si>
+    <t>gothic-hero-crouch-slash_0002_Layer-3.png</t>
+  </si>
+  <si>
+    <t>gothic-hero-crouch-slash_0006_Layer-7.png</t>
+  </si>
+  <si>
+    <t>Grenadier-Class.png</t>
+  </si>
+  <si>
     <t>Heart1.png</t>
   </si>
   <si>
+    <t>Hearts5.png</t>
+  </si>
+  <si>
+    <t>hell-beast-breath.png</t>
+  </si>
+  <si>
+    <t>nightmare-idle.png</t>
+  </si>
+  <si>
+    <t>Scarab.png</t>
+  </si>
+  <si>
+    <t>SlowTurtleIdleSide.png</t>
+  </si>
+  <si>
+    <t>sprite_0.png</t>
+  </si>
+  <si>
+    <t>sprite_1.png</t>
+  </si>
+  <si>
     <t>TopDownHouse_SmallItems.png</t>
   </si>
   <si>
-    <t>SlowTurtleIdleSide.png</t>
-  </si>
-  <si>
-    <t>Basic Humanoid Sprites 1x.png</t>
-  </si>
-  <si>
-    <t>example_16x16.png</t>
-  </si>
-  <si>
-    <t>CuriousMonkeyIdleSide.png</t>
-  </si>
-  <si>
-    <t>Hearts5.png</t>
-  </si>
-  <si>
-    <t>Base.png</t>
-  </si>
-  <si>
-    <t>example_21x27.png</t>
-  </si>
-  <si>
-    <t>gothic-hero-crouch-slash_0006_Layer-7.png</t>
-  </si>
-  <si>
-    <t>Free Sprites 1x.png</t>
-  </si>
-  <si>
-    <t>01_dish.png</t>
-  </si>
-  <si>
-    <t>07_bread.png</t>
-  </si>
-  <si>
-    <t>35_donut_dish.png</t>
-  </si>
-  <si>
-    <t>34_donut.png</t>
-  </si>
-  <si>
-    <t>44_frenchfries.png</t>
-  </si>
-  <si>
-    <t>05_apple_pie.png</t>
-  </si>
-  <si>
-    <t>32_curry.png</t>
-  </si>
-  <si>
-    <t>24_cheesepuff.png</t>
-  </si>
-  <si>
-    <t>41_eggsalad_bowl.png</t>
-  </si>
-  <si>
-    <t>18_burrito.png</t>
-  </si>
-  <si>
-    <t>13_bacon.png</t>
-  </si>
-  <si>
-    <t>28_cookies.png</t>
-  </si>
-  <si>
-    <t>36_dumplings.png</t>
-  </si>
-  <si>
-    <t>11_bun.png</t>
-  </si>
-  <si>
-    <t>09_baguette.png</t>
-  </si>
-  <si>
-    <t>38_friedegg.png</t>
-  </si>
-  <si>
-    <t>15_burger.png</t>
-  </si>
-  <si>
-    <t>99_taco.png</t>
-  </si>
-  <si>
-    <t>22_cheesecake.png</t>
-  </si>
-  <si>
-    <t>30_chocolatecake.png</t>
-  </si>
-  <si>
-    <t>20_bagel.png</t>
-  </si>
-  <si>
-    <t>40_eggsalad.png</t>
-  </si>
-  <si>
-    <t>26_chocolate.png</t>
-  </si>
-  <si>
-    <t>42_eggtart.png</t>
-  </si>
-  <si>
-    <t>sprite_1.png</t>
-  </si>
-  <si>
-    <t>sprite_0.png</t>
-  </si>
-  <si>
-    <t>ghost-shriek.png</t>
+    <t>town.png</t>
   </si>
   <si>
     <t>Wasp.png</t>
   </si>
   <si>
-    <t>hell-beast-breath.png</t>
-  </si>
-  <si>
-    <t>Scarab.png</t>
-  </si>
-  <si>
     <t>wolf-runing-cycle.png</t>
-  </si>
-  <si>
-    <t>nightmare-idle.png</t>
-  </si>
-  <si>
-    <t>Assault-Class.png</t>
-  </si>
-  <si>
-    <t>Grenadier-Class.png</t>
-  </si>
-  <si>
-    <t>gothic-hero-crouch-slash_0002_Layer-3.png</t>
-  </si>
-  <si>
-    <t>example_128x128.png</t>
-  </si>
-  <si>
-    <t>demon-idle.png</t>
-  </si>
-  <si>
-    <t>town.png</t>
-  </si>
-  <si>
-    <t>clouds.png</t>
   </si>
   <si>
     <t>Subdivisão em grupos</t>
@@ -1435,10 +1435,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1465,6 +1465,856 @@
       </c>
       <c r="E1" s="28" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1024</v>
+      </c>
+      <c r="C3">
+        <v>51.85546875</v>
+      </c>
+      <c r="D3">
+        <v>0.423007376957685</v>
+      </c>
+      <c r="E3">
+        <v>1.05317177881652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1024</v>
+      </c>
+      <c r="C4">
+        <v>84.86328125</v>
+      </c>
+      <c r="D4">
+        <v>0.413880403570753</v>
+      </c>
+      <c r="E4">
+        <v>1.06761179332417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1024</v>
+      </c>
+      <c r="C5">
+        <v>60.15625</v>
+      </c>
+      <c r="D5">
+        <v>0.488426551688462</v>
+      </c>
+      <c r="E5">
+        <v>1.032956311656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1024</v>
+      </c>
+      <c r="C6">
+        <v>96.6796875</v>
+      </c>
+      <c r="D6">
+        <v>0.410387155774515</v>
+      </c>
+      <c r="E6">
+        <v>1.08404324862503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1024</v>
+      </c>
+      <c r="C7">
+        <v>96.484375</v>
+      </c>
+      <c r="D7">
+        <v>0.3291015625</v>
+      </c>
+      <c r="E7">
+        <v>0.953505459801098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>1024</v>
+      </c>
+      <c r="C8">
+        <v>94.04296875</v>
+      </c>
+      <c r="D8">
+        <v>0.32672945800914</v>
+      </c>
+      <c r="E8">
+        <v>0.965221852878813</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1024</v>
+      </c>
+      <c r="C9">
+        <v>97.75390625</v>
+      </c>
+      <c r="D9">
+        <v>0.3681640625</v>
+      </c>
+      <c r="E9">
+        <v>1.01491607771714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1024</v>
+      </c>
+      <c r="C10">
+        <v>93.45703125</v>
+      </c>
+      <c r="D10">
+        <v>0.393845290876925</v>
+      </c>
+      <c r="E10">
+        <v>1.08780232256937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1024</v>
+      </c>
+      <c r="C11">
+        <v>99.0234375</v>
+      </c>
+      <c r="D11">
+        <v>0.391262895686547</v>
+      </c>
+      <c r="E11">
+        <v>1.08041662920656</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>1024</v>
+      </c>
+      <c r="C12">
+        <v>98.828125</v>
+      </c>
+      <c r="D12">
+        <v>0.390354671282694</v>
+      </c>
+      <c r="E12">
+        <v>1.08197432141175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1024</v>
+      </c>
+      <c r="C13">
+        <v>90.625</v>
+      </c>
+      <c r="D13">
+        <v>0.417063148789263</v>
+      </c>
+      <c r="E13">
+        <v>1.08226479973419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>1024</v>
+      </c>
+      <c r="C14">
+        <v>99.90234375</v>
+      </c>
+      <c r="D14">
+        <v>0.354815455590142</v>
+      </c>
+      <c r="E14">
+        <v>1.01197655218927</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>1024</v>
+      </c>
+      <c r="C15">
+        <v>94.43359375</v>
+      </c>
+      <c r="D15">
+        <v>0.387622849385176</v>
+      </c>
+      <c r="E15">
+        <v>1.03511985997528</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1024</v>
+      </c>
+      <c r="C16">
+        <v>98.92578125</v>
+      </c>
+      <c r="D16">
+        <v>0.362630208333333</v>
+      </c>
+      <c r="E16">
+        <v>1.03896937603622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1024</v>
+      </c>
+      <c r="C17">
+        <v>89.84375</v>
+      </c>
+      <c r="D17">
+        <v>0.388636957543592</v>
+      </c>
+      <c r="E17">
+        <v>0.969779302910118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1024</v>
+      </c>
+      <c r="C18">
+        <v>71.97265625</v>
+      </c>
+      <c r="D18">
+        <v>0.360404501872836</v>
+      </c>
+      <c r="E18">
+        <v>1.04612008988225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1024</v>
+      </c>
+      <c r="C19">
+        <v>69.23828125</v>
+      </c>
+      <c r="D19">
+        <v>0.565699640729387</v>
+      </c>
+      <c r="E19">
+        <v>1.14409291198484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>1024</v>
+      </c>
+      <c r="C20">
+        <v>95.41015625</v>
+      </c>
+      <c r="D20">
+        <v>0.390014132193755</v>
+      </c>
+      <c r="E20">
+        <v>1.09202931418287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1024</v>
+      </c>
+      <c r="C21">
+        <v>97.55859375</v>
+      </c>
+      <c r="D21">
+        <v>0.355759353376925</v>
+      </c>
+      <c r="E21">
+        <v>1.03336332402193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>1024</v>
+      </c>
+      <c r="C22">
+        <v>99.31640625</v>
+      </c>
+      <c r="D22">
+        <v>0.402488941540166</v>
+      </c>
+      <c r="E22">
+        <v>1.08861270839305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>1024</v>
+      </c>
+      <c r="C23">
+        <v>91.30859375</v>
+      </c>
+      <c r="D23">
+        <v>0.551322282893428</v>
+      </c>
+      <c r="E23">
+        <v>1.29288296346309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>1024</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>0.375165576348081</v>
+      </c>
+      <c r="E24">
+        <v>1.06873079243589</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>1024</v>
+      </c>
+      <c r="C25">
+        <v>82.91015625</v>
+      </c>
+      <c r="D25">
+        <v>0.357404979460019</v>
+      </c>
+      <c r="E25">
+        <v>0.977695706604041</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>1024</v>
+      </c>
+      <c r="C26">
+        <v>98.33984375</v>
+      </c>
+      <c r="D26">
+        <v>0.384473144338699</v>
+      </c>
+      <c r="E26">
+        <v>1.0688673126275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>8960</v>
+      </c>
+      <c r="C27">
+        <v>92.9464285714286</v>
+      </c>
+      <c r="D27">
+        <v>0.370141068362275</v>
+      </c>
+      <c r="E27">
+        <v>0.982318165343668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>360</v>
+      </c>
+      <c r="C28">
+        <v>90.2777777777778</v>
+      </c>
+      <c r="D28">
+        <v>0.48328776686219</v>
+      </c>
+      <c r="E28">
+        <v>0.99973309020982</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>169</v>
+      </c>
+      <c r="C29">
+        <v>89.9408284023669</v>
+      </c>
+      <c r="D29">
+        <v>0.46786638757839</v>
+      </c>
+      <c r="E29">
+        <v>1.22260826922813</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>45056</v>
+      </c>
+      <c r="C30">
+        <v>70.8473899147727</v>
+      </c>
+      <c r="D30">
+        <v>0.322644179071975</v>
+      </c>
+      <c r="E30">
+        <v>1.15196071025835</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>195</v>
+      </c>
+      <c r="C31">
+        <v>92.3076923076923</v>
+      </c>
+      <c r="D31">
+        <v>0.498122286927114</v>
+      </c>
+      <c r="E31">
+        <v>1.15995209164869</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>16616</v>
+      </c>
+      <c r="C32">
+        <v>73.4954260953298</v>
+      </c>
+      <c r="D32">
+        <v>0.261009246696823</v>
+      </c>
+      <c r="E32">
+        <v>0.948801573819109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>13625</v>
+      </c>
+      <c r="C33">
+        <v>89.6880733944954</v>
+      </c>
+      <c r="D33">
+        <v>0.250411547016889</v>
+      </c>
+      <c r="E33">
+        <v>0.92771001342271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>192</v>
+      </c>
+      <c r="C34">
+        <v>88.5416666666667</v>
+      </c>
+      <c r="D34">
+        <v>0.468802923785511</v>
+      </c>
+      <c r="E34">
+        <v>1.02473190906643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>567</v>
+      </c>
+      <c r="C35">
+        <v>83.0687830687831</v>
+      </c>
+      <c r="D35">
+        <v>0.428648499843317</v>
+      </c>
+      <c r="E35">
+        <v>0.993456974787705</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>960</v>
+      </c>
+      <c r="C36">
+        <v>80.7291666666667</v>
+      </c>
+      <c r="D36">
+        <v>0.50242454820416</v>
+      </c>
+      <c r="E36">
+        <v>1.08381100961621</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>1932</v>
+      </c>
+      <c r="C37">
+        <v>87.9399585921325</v>
+      </c>
+      <c r="D37">
+        <v>0.374669125774108</v>
+      </c>
+      <c r="E37">
+        <v>1.09032375335187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>10752</v>
+      </c>
+      <c r="C38">
+        <v>94.3452380952381</v>
+      </c>
+      <c r="D38">
+        <v>0.340255519284371</v>
+      </c>
+      <c r="E38">
+        <v>1.00606180576144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>957</v>
+      </c>
+      <c r="C39">
+        <v>78.7878787878788</v>
+      </c>
+      <c r="D39">
+        <v>0.348686227386312</v>
+      </c>
+      <c r="E39">
+        <v>0.996049025817482</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>8960</v>
+      </c>
+      <c r="C40">
+        <v>92.96875</v>
+      </c>
+      <c r="D40">
+        <v>0.363453409813727</v>
+      </c>
+      <c r="E40">
+        <v>0.979470798757159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>63</v>
+      </c>
+      <c r="C41">
+        <v>95.2380952380952</v>
+      </c>
+      <c r="D41">
+        <v>0.354497354497354</v>
+      </c>
+      <c r="E41">
+        <v>0.887826162104749</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>342</v>
+      </c>
+      <c r="C42">
+        <v>78.6549707602339</v>
+      </c>
+      <c r="D42">
+        <v>0.488304093567252</v>
+      </c>
+      <c r="E42">
+        <v>1.10676956739225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>2268</v>
+      </c>
+      <c r="C43">
+        <v>67.636684303351</v>
+      </c>
+      <c r="D43">
+        <v>0.448141808249823</v>
+      </c>
+      <c r="E43">
+        <v>1.03840853408364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>7371</v>
+      </c>
+      <c r="C44">
+        <v>90.7610907610908</v>
+      </c>
+      <c r="D44">
+        <v>0.205904025252076</v>
+      </c>
+      <c r="E44">
+        <v>1.11816284047538</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>6400</v>
+      </c>
+      <c r="C45">
+        <v>62.1875</v>
+      </c>
+      <c r="D45">
+        <v>0.378343814107369</v>
+      </c>
+      <c r="E45">
+        <v>0.987454838889838</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>144</v>
+      </c>
+      <c r="C46">
+        <v>96.5277777777778</v>
+      </c>
+      <c r="D46">
+        <v>0.535472467817642</v>
+      </c>
+      <c r="E46">
+        <v>1.26541971139838</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>1485</v>
+      </c>
+      <c r="C47">
+        <v>96.2962962962963</v>
+      </c>
+      <c r="D47">
+        <v>0.528264596536505</v>
+      </c>
+      <c r="E47">
+        <v>1.0236080476236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48">
+        <v>1485</v>
+      </c>
+      <c r="C48">
+        <v>92.6599326599327</v>
+      </c>
+      <c r="D48">
+        <v>0.36857903656601</v>
+      </c>
+      <c r="E48">
+        <v>1.10576755998486</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>143</v>
+      </c>
+      <c r="C49">
+        <v>88.1118881118881</v>
+      </c>
+      <c r="D49">
+        <v>0.468017949021502</v>
+      </c>
+      <c r="E49">
+        <v>0.975038398532034</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>45056</v>
+      </c>
+      <c r="C50">
+        <v>62.2181285511364</v>
+      </c>
+      <c r="D50">
+        <v>0.488304259242134</v>
+      </c>
+      <c r="E50">
+        <v>1.16560979182527</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51">
+        <v>2048</v>
+      </c>
+      <c r="C51">
+        <v>97.900390625</v>
+      </c>
+      <c r="D51">
+        <v>0.382407202656926</v>
+      </c>
+      <c r="E51">
+        <v>0.993975681131908</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>7168</v>
+      </c>
+      <c r="C52">
+        <v>45.1729910714286</v>
+      </c>
+      <c r="D52">
+        <v>0.380285999217969</v>
+      </c>
+      <c r="E52">
+        <v>0.966328699831184</v>
       </c>
     </row>
   </sheetData>
@@ -1514,7 +2364,7 @@
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B2" s="30">
         <v>63</v>
@@ -1531,7 +2381,7 @@
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B3" s="30">
         <v>143</v>
@@ -1548,7 +2398,7 @@
     </row>
     <row r="4" ht="18.75" customHeight="1" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B4" s="30">
         <v>144</v>
@@ -1565,7 +2415,7 @@
     </row>
     <row r="5" ht="18.75" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B5" s="30">
         <v>169</v>
@@ -1582,7 +2432,7 @@
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B6" s="30">
         <v>192</v>
@@ -1599,7 +2449,7 @@
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B7" s="30">
         <v>195</v>
@@ -1616,7 +2466,7 @@
     </row>
     <row r="8" ht="18.75" customHeight="1" spans="1:5">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B8" s="30">
         <v>342</v>
@@ -1633,7 +2483,7 @@
     </row>
     <row r="9" ht="18.75" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B9" s="30">
         <v>360</v>
@@ -1650,7 +2500,7 @@
     </row>
     <row r="10" ht="18.75" customHeight="1" spans="1:5">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B10" s="30">
         <v>567</v>
@@ -1667,7 +2517,7 @@
     </row>
     <row r="11" ht="18.75" customHeight="1" spans="1:5">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B11" s="30">
         <v>957</v>
@@ -1684,7 +2534,7 @@
     </row>
     <row r="12" ht="18.75" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B12" s="30">
         <v>960</v>
@@ -1701,7 +2551,7 @@
     </row>
     <row r="13" ht="18.75" customHeight="1" spans="1:5">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B13" s="30">
         <v>1024</v>
@@ -1718,7 +2568,7 @@
     </row>
     <row r="14" ht="18.75" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B14" s="30">
         <v>1024</v>
@@ -1735,7 +2585,7 @@
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:5">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" s="30">
         <v>1024</v>
@@ -1752,7 +2602,7 @@
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:5">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="30">
         <v>1024</v>
@@ -1769,7 +2619,7 @@
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:5">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B17" s="30">
         <v>1024</v>
@@ -1786,7 +2636,7 @@
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:5">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B18" s="30">
         <v>1024</v>
@@ -1803,7 +2653,7 @@
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:5">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B19" s="30">
         <v>1024</v>
@@ -1820,7 +2670,7 @@
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:5">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B20" s="30">
         <v>1024</v>
@@ -1837,7 +2687,7 @@
     </row>
     <row r="21" ht="18.75" customHeight="1" spans="1:5">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="30">
         <v>1024</v>
@@ -1854,7 +2704,7 @@
     </row>
     <row r="22" ht="18.75" customHeight="1" spans="1:5">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B22" s="30">
         <v>1024</v>
@@ -1871,7 +2721,7 @@
     </row>
     <row r="23" ht="18.75" customHeight="1" spans="1:5">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B23" s="30">
         <v>1024</v>
@@ -1888,7 +2738,7 @@
     </row>
     <row r="24" ht="18.75" customHeight="1" spans="1:8">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B24" s="30">
         <v>1024</v>
@@ -1909,7 +2759,7 @@
     </row>
     <row r="25" ht="18.75" customHeight="1" spans="1:8">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B25" s="30">
         <v>1024</v>
@@ -1930,7 +2780,7 @@
     </row>
     <row r="26" ht="18.75" customHeight="1" spans="1:8">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B26" s="30">
         <v>1024</v>
@@ -1951,7 +2801,7 @@
     </row>
     <row r="27" ht="18.75" customHeight="1" spans="1:5">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B27" s="30">
         <v>1024</v>
@@ -1968,7 +2818,7 @@
     </row>
     <row r="28" ht="18.75" customHeight="1" spans="1:5">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B28" s="30">
         <v>1024</v>
@@ -1985,7 +2835,7 @@
     </row>
     <row r="29" ht="18.75" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B29" s="30">
         <v>1024</v>
@@ -2002,7 +2852,7 @@
     </row>
     <row r="30" ht="18.75" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B30" s="30">
         <v>1024</v>
@@ -2019,7 +2869,7 @@
     </row>
     <row r="31" ht="18.75" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B31" s="30">
         <v>1024</v>
@@ -2036,7 +2886,7 @@
     </row>
     <row r="32" ht="18.75" customHeight="1" spans="1:5">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B32" s="30">
         <v>1024</v>
@@ -2053,7 +2903,7 @@
     </row>
     <row r="33" ht="18.75" customHeight="1" spans="1:5">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B33" s="30">
         <v>1024</v>
@@ -2070,7 +2920,7 @@
     </row>
     <row r="34" ht="18.75" customHeight="1" spans="1:5">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B34" s="30">
         <v>1024</v>
@@ -2087,7 +2937,7 @@
     </row>
     <row r="35" ht="18.75" customHeight="1" spans="1:5">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B35" s="30">
         <v>1024</v>
@@ -2104,7 +2954,7 @@
     </row>
     <row r="36" ht="18.75" customHeight="1" spans="1:5">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B36" s="30">
         <v>1024</v>
@@ -2121,7 +2971,7 @@
     </row>
     <row r="37" ht="18.75" customHeight="1" spans="1:5">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B37" s="30">
         <v>1485</v>
@@ -2138,7 +2988,7 @@
     </row>
     <row r="38" ht="18.75" customHeight="1" spans="1:5">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B38" s="30">
         <v>1485</v>
@@ -2155,7 +3005,7 @@
     </row>
     <row r="39" ht="18.75" customHeight="1" spans="1:5">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B39" s="30">
         <v>1932</v>
@@ -2172,7 +3022,7 @@
     </row>
     <row r="40" ht="18.75" customHeight="1" spans="1:5">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B40" s="30">
         <v>2048</v>
@@ -2189,7 +3039,7 @@
     </row>
     <row r="41" ht="18.75" customHeight="1" spans="1:5">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B41" s="30">
         <v>2268</v>
@@ -2206,7 +3056,7 @@
     </row>
     <row r="42" ht="18.75" customHeight="1" spans="1:5">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B42" s="30">
         <v>6400</v>
@@ -2223,7 +3073,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:5">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B43" s="30">
         <v>7168</v>
@@ -2240,7 +3090,7 @@
     </row>
     <row r="44" ht="18.75" customHeight="1" spans="1:5">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="30">
         <v>7371</v>
@@ -2257,7 +3107,7 @@
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:5">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B45" s="30">
         <v>8960</v>
@@ -2274,7 +3124,7 @@
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:5">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B46" s="30">
         <v>8960</v>
@@ -2291,7 +3141,7 @@
     </row>
     <row r="47" ht="18.75" customHeight="1" spans="1:5">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B47" s="30">
         <v>10752</v>
@@ -2308,7 +3158,7 @@
     </row>
     <row r="48" ht="18.75" customHeight="1" spans="1:5">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B48" s="30">
         <v>13625</v>
@@ -2325,7 +3175,7 @@
     </row>
     <row r="49" ht="18.75" customHeight="1" spans="1:5">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B49" s="30">
         <v>16616</v>
@@ -2342,7 +3192,7 @@
     </row>
     <row r="50" ht="18.75" customHeight="1" spans="1:5">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" s="30">
         <v>45056</v>
@@ -2359,7 +3209,7 @@
     </row>
     <row r="51" ht="18.75" customHeight="1" spans="1:5">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B51" s="30">
         <v>45056</v>
@@ -3642,7 +4492,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B54">
         <v>1024</v>
@@ -3659,7 +4509,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B55">
         <v>1024</v>

</xml_diff>

<commit_message>
Alteração dos dados para receber outros formatos de análise
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7500"/>
+    <workbookView windowWidth="20490" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>Imagem</t>
   </si>
@@ -61,163 +61,172 @@
     <t>Quantidade de pixels</t>
   </si>
   <si>
+    <t>Tamanho Imagem</t>
+  </si>
+  <si>
     <t>porcentagem de acerto</t>
   </si>
   <si>
     <t>MSE</t>
   </si>
   <si>
+    <t>R Squared</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
     <t>Erro quadrático</t>
   </si>
   <si>
+    <t>Heart1.png</t>
+  </si>
+  <si>
+    <t>TopDownHouse_SmallItems.png</t>
+  </si>
+  <si>
+    <t>SlowTurtleIdleSide.png</t>
+  </si>
+  <si>
+    <t>Basic Humanoid Sprites 1x.png</t>
+  </si>
+  <si>
+    <t>example_16x16.png</t>
+  </si>
+  <si>
+    <t>CuriousMonkeyIdleSide.png</t>
+  </si>
+  <si>
+    <t>Hearts5.png</t>
+  </si>
+  <si>
+    <t>Base.png</t>
+  </si>
+  <si>
+    <t>example_21x27.png</t>
+  </si>
+  <si>
+    <t>gothic-hero-crouch-slash_0006_Layer-7.png</t>
+  </si>
+  <si>
+    <t>Free Sprites 1x.png</t>
+  </si>
+  <si>
     <t>01_dish.png</t>
   </si>
   <si>
+    <t>07_bread.png</t>
+  </si>
+  <si>
+    <t>35_donut_dish.png</t>
+  </si>
+  <si>
+    <t>34_donut.png</t>
+  </si>
+  <si>
+    <t>44_frenchfries.png</t>
+  </si>
+  <si>
     <t>05_apple_pie.png</t>
   </si>
   <si>
-    <t>07_bread.png</t>
+    <t>32_curry.png</t>
+  </si>
+  <si>
+    <t>24_cheesepuff.png</t>
+  </si>
+  <si>
+    <t>41_eggsalad_bowl.png</t>
+  </si>
+  <si>
+    <t>18_burrito.png</t>
+  </si>
+  <si>
+    <t>13_bacon.png</t>
+  </si>
+  <si>
+    <t>28_cookies.png</t>
+  </si>
+  <si>
+    <t>36_dumplings.png</t>
+  </si>
+  <si>
+    <t>11_bun.png</t>
   </si>
   <si>
     <t>09_baguette.png</t>
   </si>
   <si>
-    <t>11_bun.png</t>
-  </si>
-  <si>
-    <t>13_bacon.png</t>
+    <t>38_friedegg.png</t>
   </si>
   <si>
     <t>15_burger.png</t>
   </si>
   <si>
-    <t>18_burrito.png</t>
+    <t>99_taco.png</t>
+  </si>
+  <si>
+    <t>22_cheesecake.png</t>
+  </si>
+  <si>
+    <t>30_chocolatecake.png</t>
   </si>
   <si>
     <t>20_bagel.png</t>
   </si>
   <si>
-    <t>22_cheesecake.png</t>
-  </si>
-  <si>
-    <t>24_cheesepuff.png</t>
+    <t>40_eggsalad.png</t>
   </si>
   <si>
     <t>26_chocolate.png</t>
   </si>
   <si>
-    <t>28_cookies.png</t>
-  </si>
-  <si>
-    <t>30_chocolatecake.png</t>
-  </si>
-  <si>
-    <t>32_curry.png</t>
-  </si>
-  <si>
-    <t>34_donut.png</t>
-  </si>
-  <si>
-    <t>35_donut_dish.png</t>
-  </si>
-  <si>
-    <t>36_dumplings.png</t>
-  </si>
-  <si>
-    <t>38_friedegg.png</t>
-  </si>
-  <si>
-    <t>40_eggsalad.png</t>
-  </si>
-  <si>
-    <t>41_eggsalad_bowl.png</t>
-  </si>
-  <si>
     <t>42_eggtart.png</t>
   </si>
   <si>
-    <t>44_frenchfries.png</t>
-  </si>
-  <si>
-    <t>99_taco.png</t>
+    <t>sprite_1.png</t>
+  </si>
+  <si>
+    <t>sprite_0.png</t>
+  </si>
+  <si>
+    <t>ghost-shriek.png</t>
+  </si>
+  <si>
+    <t>Wasp.png</t>
+  </si>
+  <si>
+    <t>hell-beast-breath.png</t>
+  </si>
+  <si>
+    <t>Scarab.png</t>
+  </si>
+  <si>
+    <t>wolf-runing-cycle.png</t>
+  </si>
+  <si>
+    <t>nightmare-idle.png</t>
   </si>
   <si>
     <t>Assault-Class.png</t>
   </si>
   <si>
-    <t>Base.png</t>
-  </si>
-  <si>
-    <t>Basic Humanoid Sprites 1x.png</t>
+    <t>Grenadier-Class.png</t>
+  </si>
+  <si>
+    <t>gothic-hero-crouch-slash_0002_Layer-3.png</t>
+  </si>
+  <si>
+    <t>example_128x128.png</t>
+  </si>
+  <si>
+    <t>demon-idle.png</t>
+  </si>
+  <si>
+    <t>town.png</t>
   </si>
   <si>
     <t>clouds.png</t>
-  </si>
-  <si>
-    <t>CuriousMonkeyIdleSide.png</t>
-  </si>
-  <si>
-    <t>demon-idle.png</t>
-  </si>
-  <si>
-    <t>example_128x128.png</t>
-  </si>
-  <si>
-    <t>example_16x16.png</t>
-  </si>
-  <si>
-    <t>example_21x27.png</t>
-  </si>
-  <si>
-    <t>Free Sprites 1x.png</t>
-  </si>
-  <si>
-    <t>ghost-shriek.png</t>
-  </si>
-  <si>
-    <t>gothic-hero-crouch-slash_0002_Layer-3.png</t>
-  </si>
-  <si>
-    <t>gothic-hero-crouch-slash_0006_Layer-7.png</t>
-  </si>
-  <si>
-    <t>Grenadier-Class.png</t>
-  </si>
-  <si>
-    <t>Heart1.png</t>
-  </si>
-  <si>
-    <t>Hearts5.png</t>
-  </si>
-  <si>
-    <t>hell-beast-breath.png</t>
-  </si>
-  <si>
-    <t>nightmare-idle.png</t>
-  </si>
-  <si>
-    <t>Scarab.png</t>
-  </si>
-  <si>
-    <t>SlowTurtleIdleSide.png</t>
-  </si>
-  <si>
-    <t>sprite_0.png</t>
-  </si>
-  <si>
-    <t>sprite_1.png</t>
-  </si>
-  <si>
-    <t>TopDownHouse_SmallItems.png</t>
-  </si>
-  <si>
-    <t>town.png</t>
-  </si>
-  <si>
-    <t>Wasp.png</t>
-  </si>
-  <si>
-    <t>wolf-runing-cycle.png</t>
   </si>
   <si>
     <t>Subdivisão em grupos</t>
@@ -1435,22 +1444,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A3" sqref="A3:E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="8.71428571428571" customWidth="1"/>
+    <col min="1" max="1" width="43.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="5.28571428571429" customWidth="1"/>
-    <col min="5" max="5" width="15.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="23.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="12.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="10.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="8.85714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1466,855 +1477,11 @@
       <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>1024</v>
-      </c>
-      <c r="C3">
-        <v>51.85546875</v>
-      </c>
-      <c r="D3">
-        <v>0.423007376957685</v>
-      </c>
-      <c r="E3">
-        <v>1.05317177881652</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1024</v>
-      </c>
-      <c r="C4">
-        <v>84.86328125</v>
-      </c>
-      <c r="D4">
-        <v>0.413880403570753</v>
-      </c>
-      <c r="E4">
-        <v>1.06761179332417</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>1024</v>
-      </c>
-      <c r="C5">
-        <v>60.15625</v>
-      </c>
-      <c r="D5">
-        <v>0.488426551688462</v>
-      </c>
-      <c r="E5">
-        <v>1.032956311656</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1024</v>
-      </c>
-      <c r="C6">
-        <v>96.6796875</v>
-      </c>
-      <c r="D6">
-        <v>0.410387155774515</v>
-      </c>
-      <c r="E6">
-        <v>1.08404324862503</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>1024</v>
-      </c>
-      <c r="C7">
-        <v>96.484375</v>
-      </c>
-      <c r="D7">
-        <v>0.3291015625</v>
-      </c>
-      <c r="E7">
-        <v>0.953505459801098</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>1024</v>
-      </c>
-      <c r="C8">
-        <v>94.04296875</v>
-      </c>
-      <c r="D8">
-        <v>0.32672945800914</v>
-      </c>
-      <c r="E8">
-        <v>0.965221852878813</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>1024</v>
-      </c>
-      <c r="C9">
-        <v>97.75390625</v>
-      </c>
-      <c r="D9">
-        <v>0.3681640625</v>
-      </c>
-      <c r="E9">
-        <v>1.01491607771714</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>1024</v>
-      </c>
-      <c r="C10">
-        <v>93.45703125</v>
-      </c>
-      <c r="D10">
-        <v>0.393845290876925</v>
-      </c>
-      <c r="E10">
-        <v>1.08780232256937</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>1024</v>
-      </c>
-      <c r="C11">
-        <v>99.0234375</v>
-      </c>
-      <c r="D11">
-        <v>0.391262895686547</v>
-      </c>
-      <c r="E11">
-        <v>1.08041662920656</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>1024</v>
-      </c>
-      <c r="C12">
-        <v>98.828125</v>
-      </c>
-      <c r="D12">
-        <v>0.390354671282694</v>
-      </c>
-      <c r="E12">
-        <v>1.08197432141175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>1024</v>
-      </c>
-      <c r="C13">
-        <v>90.625</v>
-      </c>
-      <c r="D13">
-        <v>0.417063148789263</v>
-      </c>
-      <c r="E13">
-        <v>1.08226479973419</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>1024</v>
-      </c>
-      <c r="C14">
-        <v>99.90234375</v>
-      </c>
-      <c r="D14">
-        <v>0.354815455590142</v>
-      </c>
-      <c r="E14">
-        <v>1.01197655218927</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>1024</v>
-      </c>
-      <c r="C15">
-        <v>94.43359375</v>
-      </c>
-      <c r="D15">
-        <v>0.387622849385176</v>
-      </c>
-      <c r="E15">
-        <v>1.03511985997528</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>1024</v>
-      </c>
-      <c r="C16">
-        <v>98.92578125</v>
-      </c>
-      <c r="D16">
-        <v>0.362630208333333</v>
-      </c>
-      <c r="E16">
-        <v>1.03896937603622</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>1024</v>
-      </c>
-      <c r="C17">
-        <v>89.84375</v>
-      </c>
-      <c r="D17">
-        <v>0.388636957543592</v>
-      </c>
-      <c r="E17">
-        <v>0.969779302910118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>1024</v>
-      </c>
-      <c r="C18">
-        <v>71.97265625</v>
-      </c>
-      <c r="D18">
-        <v>0.360404501872836</v>
-      </c>
-      <c r="E18">
-        <v>1.04612008988225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>1024</v>
-      </c>
-      <c r="C19">
-        <v>69.23828125</v>
-      </c>
-      <c r="D19">
-        <v>0.565699640729387</v>
-      </c>
-      <c r="E19">
-        <v>1.14409291198484</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>1024</v>
-      </c>
-      <c r="C20">
-        <v>95.41015625</v>
-      </c>
-      <c r="D20">
-        <v>0.390014132193755</v>
-      </c>
-      <c r="E20">
-        <v>1.09202931418287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>1024</v>
-      </c>
-      <c r="C21">
-        <v>97.55859375</v>
-      </c>
-      <c r="D21">
-        <v>0.355759353376925</v>
-      </c>
-      <c r="E21">
-        <v>1.03336332402193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>1024</v>
-      </c>
-      <c r="C22">
-        <v>99.31640625</v>
-      </c>
-      <c r="D22">
-        <v>0.402488941540166</v>
-      </c>
-      <c r="E22">
-        <v>1.08861270839305</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>1024</v>
-      </c>
-      <c r="C23">
-        <v>91.30859375</v>
-      </c>
-      <c r="D23">
-        <v>0.551322282893428</v>
-      </c>
-      <c r="E23">
-        <v>1.29288296346309</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>1024</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-      <c r="D24">
-        <v>0.375165576348081</v>
-      </c>
-      <c r="E24">
-        <v>1.06873079243589</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>1024</v>
-      </c>
-      <c r="C25">
-        <v>82.91015625</v>
-      </c>
-      <c r="D25">
-        <v>0.357404979460019</v>
-      </c>
-      <c r="E25">
-        <v>0.977695706604041</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>1024</v>
-      </c>
-      <c r="C26">
-        <v>98.33984375</v>
-      </c>
-      <c r="D26">
-        <v>0.384473144338699</v>
-      </c>
-      <c r="E26">
-        <v>1.0688673126275</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>8960</v>
-      </c>
-      <c r="C27">
-        <v>92.9464285714286</v>
-      </c>
-      <c r="D27">
-        <v>0.370141068362275</v>
-      </c>
-      <c r="E27">
-        <v>0.982318165343668</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>360</v>
-      </c>
-      <c r="C28">
-        <v>90.2777777777778</v>
-      </c>
-      <c r="D28">
-        <v>0.48328776686219</v>
-      </c>
-      <c r="E28">
-        <v>0.99973309020982</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29">
-        <v>169</v>
-      </c>
-      <c r="C29">
-        <v>89.9408284023669</v>
-      </c>
-      <c r="D29">
-        <v>0.46786638757839</v>
-      </c>
-      <c r="E29">
-        <v>1.22260826922813</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>45056</v>
-      </c>
-      <c r="C30">
-        <v>70.8473899147727</v>
-      </c>
-      <c r="D30">
-        <v>0.322644179071975</v>
-      </c>
-      <c r="E30">
-        <v>1.15196071025835</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31">
-        <v>195</v>
-      </c>
-      <c r="C31">
-        <v>92.3076923076923</v>
-      </c>
-      <c r="D31">
-        <v>0.498122286927114</v>
-      </c>
-      <c r="E31">
-        <v>1.15995209164869</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>16616</v>
-      </c>
-      <c r="C32">
-        <v>73.4954260953298</v>
-      </c>
-      <c r="D32">
-        <v>0.261009246696823</v>
-      </c>
-      <c r="E32">
-        <v>0.948801573819109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33">
-        <v>13625</v>
-      </c>
-      <c r="C33">
-        <v>89.6880733944954</v>
-      </c>
-      <c r="D33">
-        <v>0.250411547016889</v>
-      </c>
-      <c r="E33">
-        <v>0.92771001342271</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34">
-        <v>192</v>
-      </c>
-      <c r="C34">
-        <v>88.5416666666667</v>
-      </c>
-      <c r="D34">
-        <v>0.468802923785511</v>
-      </c>
-      <c r="E34">
-        <v>1.02473190906643</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>567</v>
-      </c>
-      <c r="C35">
-        <v>83.0687830687831</v>
-      </c>
-      <c r="D35">
-        <v>0.428648499843317</v>
-      </c>
-      <c r="E35">
-        <v>0.993456974787705</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>960</v>
-      </c>
-      <c r="C36">
-        <v>80.7291666666667</v>
-      </c>
-      <c r="D36">
-        <v>0.50242454820416</v>
-      </c>
-      <c r="E36">
-        <v>1.08381100961621</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37">
-        <v>1932</v>
-      </c>
-      <c r="C37">
-        <v>87.9399585921325</v>
-      </c>
-      <c r="D37">
-        <v>0.374669125774108</v>
-      </c>
-      <c r="E37">
-        <v>1.09032375335187</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38">
-        <v>10752</v>
-      </c>
-      <c r="C38">
-        <v>94.3452380952381</v>
-      </c>
-      <c r="D38">
-        <v>0.340255519284371</v>
-      </c>
-      <c r="E38">
-        <v>1.00606180576144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39">
-        <v>957</v>
-      </c>
-      <c r="C39">
-        <v>78.7878787878788</v>
-      </c>
-      <c r="D39">
-        <v>0.348686227386312</v>
-      </c>
-      <c r="E39">
-        <v>0.996049025817482</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40">
-        <v>8960</v>
-      </c>
-      <c r="C40">
-        <v>92.96875</v>
-      </c>
-      <c r="D40">
-        <v>0.363453409813727</v>
-      </c>
-      <c r="E40">
-        <v>0.979470798757159</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41">
-        <v>63</v>
-      </c>
-      <c r="C41">
-        <v>95.2380952380952</v>
-      </c>
-      <c r="D41">
-        <v>0.354497354497354</v>
-      </c>
-      <c r="E41">
-        <v>0.887826162104749</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42">
-        <v>342</v>
-      </c>
-      <c r="C42">
-        <v>78.6549707602339</v>
-      </c>
-      <c r="D42">
-        <v>0.488304093567252</v>
-      </c>
-      <c r="E42">
-        <v>1.10676956739225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43">
-        <v>2268</v>
-      </c>
-      <c r="C43">
-        <v>67.636684303351</v>
-      </c>
-      <c r="D43">
-        <v>0.448141808249823</v>
-      </c>
-      <c r="E43">
-        <v>1.03840853408364</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44">
-        <v>7371</v>
-      </c>
-      <c r="C44">
-        <v>90.7610907610908</v>
-      </c>
-      <c r="D44">
-        <v>0.205904025252076</v>
-      </c>
-      <c r="E44">
-        <v>1.11816284047538</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45">
-        <v>6400</v>
-      </c>
-      <c r="C45">
-        <v>62.1875</v>
-      </c>
-      <c r="D45">
-        <v>0.378343814107369</v>
-      </c>
-      <c r="E45">
-        <v>0.987454838889838</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46">
-        <v>144</v>
-      </c>
-      <c r="C46">
-        <v>96.5277777777778</v>
-      </c>
-      <c r="D46">
-        <v>0.535472467817642</v>
-      </c>
-      <c r="E46">
-        <v>1.26541971139838</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47">
-        <v>1485</v>
-      </c>
-      <c r="C47">
-        <v>96.2962962962963</v>
-      </c>
-      <c r="D47">
-        <v>0.528264596536505</v>
-      </c>
-      <c r="E47">
-        <v>1.0236080476236</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48">
-        <v>1485</v>
-      </c>
-      <c r="C48">
-        <v>92.6599326599327</v>
-      </c>
-      <c r="D48">
-        <v>0.36857903656601</v>
-      </c>
-      <c r="E48">
-        <v>1.10576755998486</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49">
-        <v>143</v>
-      </c>
-      <c r="C49">
-        <v>88.1118881118881</v>
-      </c>
-      <c r="D49">
-        <v>0.468017949021502</v>
-      </c>
-      <c r="E49">
-        <v>0.975038398532034</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50">
-        <v>45056</v>
-      </c>
-      <c r="C50">
-        <v>62.2181285511364</v>
-      </c>
-      <c r="D50">
-        <v>0.488304259242134</v>
-      </c>
-      <c r="E50">
-        <v>1.16560979182527</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51">
-        <v>2048</v>
-      </c>
-      <c r="C51">
-        <v>97.900390625</v>
-      </c>
-      <c r="D51">
-        <v>0.382407202656926</v>
-      </c>
-      <c r="E51">
-        <v>0.993975681131908</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52">
-        <v>7168</v>
-      </c>
-      <c r="C52">
-        <v>45.1729910714286</v>
-      </c>
-      <c r="D52">
-        <v>0.380285999217969</v>
-      </c>
-      <c r="E52">
-        <v>0.966328699831184</v>
       </c>
     </row>
   </sheetData>
@@ -2353,18 +1520,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:5">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B2" s="30">
         <v>63</v>
@@ -2381,7 +1548,7 @@
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B3" s="30">
         <v>143</v>
@@ -2398,7 +1565,7 @@
     </row>
     <row r="4" ht="18.75" customHeight="1" spans="1:5">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B4" s="30">
         <v>144</v>
@@ -2415,7 +1582,7 @@
     </row>
     <row r="5" ht="18.75" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B5" s="30">
         <v>169</v>
@@ -2432,7 +1599,7 @@
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:5">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B6" s="30">
         <v>192</v>
@@ -2449,7 +1616,7 @@
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:5">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B7" s="30">
         <v>195</v>
@@ -2466,7 +1633,7 @@
     </row>
     <row r="8" ht="18.75" customHeight="1" spans="1:5">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B8" s="30">
         <v>342</v>
@@ -2483,7 +1650,7 @@
     </row>
     <row r="9" ht="18.75" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B9" s="30">
         <v>360</v>
@@ -2500,7 +1667,7 @@
     </row>
     <row r="10" ht="18.75" customHeight="1" spans="1:5">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B10" s="30">
         <v>567</v>
@@ -2517,7 +1684,7 @@
     </row>
     <row r="11" ht="18.75" customHeight="1" spans="1:5">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B11" s="30">
         <v>957</v>
@@ -2534,7 +1701,7 @@
     </row>
     <row r="12" ht="18.75" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B12" s="30">
         <v>960</v>
@@ -2551,7 +1718,7 @@
     </row>
     <row r="13" ht="18.75" customHeight="1" spans="1:5">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B13" s="30">
         <v>1024</v>
@@ -2568,7 +1735,7 @@
     </row>
     <row r="14" ht="18.75" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B14" s="30">
         <v>1024</v>
@@ -2602,7 +1769,7 @@
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:5">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="30">
         <v>1024</v>
@@ -2619,7 +1786,7 @@
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:5">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B17" s="30">
         <v>1024</v>
@@ -2636,7 +1803,7 @@
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:5">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B18" s="30">
         <v>1024</v>
@@ -2653,7 +1820,7 @@
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:5">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B19" s="30">
         <v>1024</v>
@@ -2670,7 +1837,7 @@
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:5">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B20" s="30">
         <v>1024</v>
@@ -2687,7 +1854,7 @@
     </row>
     <row r="21" ht="18.75" customHeight="1" spans="1:5">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" s="30">
         <v>1024</v>
@@ -2704,7 +1871,7 @@
     </row>
     <row r="22" ht="18.75" customHeight="1" spans="1:5">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B22" s="30">
         <v>1024</v>
@@ -2721,7 +1888,7 @@
     </row>
     <row r="23" ht="18.75" customHeight="1" spans="1:5">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B23" s="30">
         <v>1024</v>
@@ -2738,7 +1905,7 @@
     </row>
     <row r="24" ht="18.75" customHeight="1" spans="1:8">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B24" s="30">
         <v>1024</v>
@@ -2759,7 +1926,7 @@
     </row>
     <row r="25" ht="18.75" customHeight="1" spans="1:8">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B25" s="30">
         <v>1024</v>
@@ -2780,7 +1947,7 @@
     </row>
     <row r="26" ht="18.75" customHeight="1" spans="1:8">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B26" s="30">
         <v>1024</v>
@@ -2801,7 +1968,7 @@
     </row>
     <row r="27" ht="18.75" customHeight="1" spans="1:5">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B27" s="30">
         <v>1024</v>
@@ -2818,7 +1985,7 @@
     </row>
     <row r="28" ht="18.75" customHeight="1" spans="1:5">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B28" s="30">
         <v>1024</v>
@@ -2835,7 +2002,7 @@
     </row>
     <row r="29" ht="18.75" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B29" s="30">
         <v>1024</v>
@@ -2852,7 +2019,7 @@
     </row>
     <row r="30" ht="18.75" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B30" s="30">
         <v>1024</v>
@@ -2869,7 +2036,7 @@
     </row>
     <row r="31" ht="18.75" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B31" s="30">
         <v>1024</v>
@@ -2886,7 +2053,7 @@
     </row>
     <row r="32" ht="18.75" customHeight="1" spans="1:5">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B32" s="30">
         <v>1024</v>
@@ -2903,7 +2070,7 @@
     </row>
     <row r="33" ht="18.75" customHeight="1" spans="1:5">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B33" s="30">
         <v>1024</v>
@@ -2920,7 +2087,7 @@
     </row>
     <row r="34" ht="18.75" customHeight="1" spans="1:5">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B34" s="30">
         <v>1024</v>
@@ -2937,7 +2104,7 @@
     </row>
     <row r="35" ht="18.75" customHeight="1" spans="1:5">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B35" s="30">
         <v>1024</v>
@@ -2954,7 +2121,7 @@
     </row>
     <row r="36" ht="18.75" customHeight="1" spans="1:5">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B36" s="30">
         <v>1024</v>
@@ -2971,7 +2138,7 @@
     </row>
     <row r="37" ht="18.75" customHeight="1" spans="1:5">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B37" s="30">
         <v>1485</v>
@@ -2988,7 +2155,7 @@
     </row>
     <row r="38" ht="18.75" customHeight="1" spans="1:5">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B38" s="30">
         <v>1485</v>
@@ -3005,7 +2172,7 @@
     </row>
     <row r="39" ht="18.75" customHeight="1" spans="1:5">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B39" s="30">
         <v>1932</v>
@@ -3022,7 +2189,7 @@
     </row>
     <row r="40" ht="18.75" customHeight="1" spans="1:5">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B40" s="30">
         <v>2048</v>
@@ -3039,7 +2206,7 @@
     </row>
     <row r="41" ht="18.75" customHeight="1" spans="1:5">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B41" s="30">
         <v>2268</v>
@@ -3056,7 +2223,7 @@
     </row>
     <row r="42" ht="18.75" customHeight="1" spans="1:5">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B42" s="30">
         <v>6400</v>
@@ -3073,7 +2240,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:5">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B43" s="30">
         <v>7168</v>
@@ -3090,7 +2257,7 @@
     </row>
     <row r="44" ht="18.75" customHeight="1" spans="1:5">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B44" s="30">
         <v>7371</v>
@@ -3107,7 +2274,7 @@
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:5">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B45" s="30">
         <v>8960</v>
@@ -3124,7 +2291,7 @@
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:5">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B46" s="30">
         <v>8960</v>
@@ -3141,7 +2308,7 @@
     </row>
     <row r="47" ht="18.75" customHeight="1" spans="1:5">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B47" s="30">
         <v>10752</v>
@@ -3158,7 +2325,7 @@
     </row>
     <row r="48" ht="18.75" customHeight="1" spans="1:5">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B48" s="30">
         <v>13625</v>
@@ -3175,7 +2342,7 @@
     </row>
     <row r="49" ht="18.75" customHeight="1" spans="1:5">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B49" s="30">
         <v>16616</v>
@@ -3192,7 +2359,7 @@
     </row>
     <row r="50" ht="18.75" customHeight="1" spans="1:5">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B50" s="30">
         <v>45056</v>
@@ -3209,7 +2376,7 @@
     </row>
     <row r="51" ht="18.75" customHeight="1" spans="1:5">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B51" s="30">
         <v>45056</v>
@@ -3252,39 +2419,39 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3304,7 +2471,7 @@
         <v>63</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" s="8">
         <f>MEDIAN(principal!D2:D12)</f>
@@ -3337,7 +2504,7 @@
         <v>143</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H4" s="8">
         <f>MEDIAN(principal!E2:E12)</f>
@@ -3370,7 +2537,7 @@
         <v>144</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H5" s="8">
         <f>MEDIAN(principal!C2:C12)</f>
@@ -3420,19 +2587,19 @@
         <v>192</v>
       </c>
       <c r="G7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3452,7 +2619,7 @@
         <v>195</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H8" s="10">
         <f>MEDIAN(principal!D13:D41)</f>
@@ -3485,7 +2652,7 @@
         <v>342</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H9" s="10">
         <f>MEDIAN(principal!E13:E41)</f>
@@ -3518,7 +2685,7 @@
         <v>360</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H10" s="10">
         <f>MEDIAN(principal!C13:C41)</f>
@@ -3568,19 +2735,19 @@
         <v>957</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -3600,7 +2767,7 @@
         <v>960</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="13">
         <f>MEDIAN(principal!D42:D46)</f>
@@ -3633,7 +2800,7 @@
         <v>1024</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H14" s="13">
         <f>MEDIAN(principal!E42:E46)</f>
@@ -3666,7 +2833,7 @@
         <v>1024</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H15" s="13">
         <f>MEDIAN(principal!C42:C46)</f>
@@ -3716,19 +2883,19 @@
         <v>1024</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -3748,7 +2915,7 @@
         <v>1024</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18" s="16">
         <f>MEDIAN(principal!D47:D51)</f>
@@ -3781,7 +2948,7 @@
         <v>1024</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H19" s="16">
         <f>MEDIAN(principal!E47:E51)</f>
@@ -3814,7 +2981,7 @@
         <v>1024</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H20" s="16">
         <f>MEDIAN(principal!C47:C51)</f>
@@ -4204,7 +3371,7 @@
         <v>2268</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -4279,16 +3446,16 @@
         <v>8960</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -4492,7 +3659,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B54">
         <v>1024</v>
@@ -4509,7 +3676,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B55">
         <v>1024</v>

</xml_diff>

<commit_message>
Dados carregados e main atuaizada
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7050"/>
+    <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="102">
   <si>
     <t>Imagem</t>
   </si>
@@ -70,163 +70,232 @@
     <t>MSE</t>
   </si>
   <si>
-    <t>R Squared</t>
-  </si>
-  <si>
-    <t>F1 Score</t>
+    <t>NCC</t>
+  </si>
+  <si>
+    <t>01_dish.png</t>
+  </si>
+  <si>
+    <t>32x32</t>
+  </si>
+  <si>
+    <t>05_apple_pie.png</t>
+  </si>
+  <si>
+    <t>07_bread.png</t>
+  </si>
+  <si>
+    <t>09_baguette.png</t>
+  </si>
+  <si>
+    <t>11_bun.png</t>
+  </si>
+  <si>
+    <t>13_bacon.png</t>
+  </si>
+  <si>
+    <t>15_burger.png</t>
+  </si>
+  <si>
+    <t>18_burrito.png</t>
+  </si>
+  <si>
+    <t>20_bagel.png</t>
+  </si>
+  <si>
+    <t>22_cheesecake.png</t>
+  </si>
+  <si>
+    <t>24_cheesepuff.png</t>
+  </si>
+  <si>
+    <t>26_chocolate.png</t>
+  </si>
+  <si>
+    <t>28_cookies.png</t>
+  </si>
+  <si>
+    <t>30_chocolatecake.png</t>
+  </si>
+  <si>
+    <t>32_curry.png</t>
+  </si>
+  <si>
+    <t>34_donut.png</t>
+  </si>
+  <si>
+    <t>35_donut_dish.png</t>
+  </si>
+  <si>
+    <t>36_dumplings.png</t>
+  </si>
+  <si>
+    <t>38_friedegg.png</t>
+  </si>
+  <si>
+    <t>40_eggsalad.png</t>
+  </si>
+  <si>
+    <t>41_eggsalad_bowl.png</t>
+  </si>
+  <si>
+    <t>42_eggtart.png</t>
+  </si>
+  <si>
+    <t>44_frenchfries.png</t>
+  </si>
+  <si>
+    <t>99_taco.png</t>
+  </si>
+  <si>
+    <t>Assault-Class.png</t>
+  </si>
+  <si>
+    <t>112x80</t>
+  </si>
+  <si>
+    <t>Base.png</t>
+  </si>
+  <si>
+    <t>18x20</t>
+  </si>
+  <si>
+    <t>Basic Humanoid Sprites 1x.png</t>
+  </si>
+  <si>
+    <t>13x13</t>
+  </si>
+  <si>
+    <t>clouds.png</t>
+  </si>
+  <si>
+    <t>176x256</t>
+  </si>
+  <si>
+    <t>CuriousMonkeyIdleSide.png</t>
+  </si>
+  <si>
+    <t>15x13</t>
+  </si>
+  <si>
+    <t>demon-idle.png</t>
+  </si>
+  <si>
+    <t>124x134</t>
+  </si>
+  <si>
+    <t>example_128x128.png</t>
+  </si>
+  <si>
+    <t>125x109</t>
+  </si>
+  <si>
+    <t>example_16x16.png</t>
+  </si>
+  <si>
+    <t>12x16</t>
+  </si>
+  <si>
+    <t>example_21x27.png</t>
+  </si>
+  <si>
+    <t>21x27</t>
+  </si>
+  <si>
+    <t>Free Sprites 1x.png</t>
+  </si>
+  <si>
+    <t>30x32</t>
+  </si>
+  <si>
+    <t>ghost-shriek.png</t>
+  </si>
+  <si>
+    <t>42x46</t>
+  </si>
+  <si>
+    <t>gothic-hero-crouch-slash_0002_Layer-3.png</t>
+  </si>
+  <si>
+    <t>96x112</t>
+  </si>
+  <si>
+    <t>gothic-hero-crouch-slash_0006_Layer-7.png</t>
+  </si>
+  <si>
+    <t>29x33</t>
+  </si>
+  <si>
+    <t>Grenadier-Class.png</t>
+  </si>
+  <si>
+    <t>Heart1.png</t>
+  </si>
+  <si>
+    <t>7x9</t>
+  </si>
+  <si>
+    <t>Hearts5.png</t>
+  </si>
+  <si>
+    <t>18x19</t>
+  </si>
+  <si>
+    <t>hell-beast-breath.png</t>
+  </si>
+  <si>
+    <t>54x42</t>
+  </si>
+  <si>
+    <t>nightmare-idle.png</t>
+  </si>
+  <si>
+    <t>81x91</t>
+  </si>
+  <si>
+    <t>Scarab.png</t>
+  </si>
+  <si>
+    <t>80x80</t>
+  </si>
+  <si>
+    <t>SlowTurtleIdleSide.png</t>
+  </si>
+  <si>
+    <t>9x16</t>
+  </si>
+  <si>
+    <t>sprite_0.png</t>
+  </si>
+  <si>
+    <t>55x27</t>
+  </si>
+  <si>
+    <t>sprite_1.png</t>
+  </si>
+  <si>
+    <t>TopDownHouse_SmallItems.png</t>
+  </si>
+  <si>
+    <t>11x13</t>
+  </si>
+  <si>
+    <t>town.png</t>
+  </si>
+  <si>
+    <t>Wasp.png</t>
+  </si>
+  <si>
+    <t>16x128</t>
+  </si>
+  <si>
+    <t>wolf-runing-cycle.png</t>
+  </si>
+  <si>
+    <t>32x224</t>
   </si>
   <si>
     <t>Erro quadrático</t>
-  </si>
-  <si>
-    <t>Heart1.png</t>
-  </si>
-  <si>
-    <t>TopDownHouse_SmallItems.png</t>
-  </si>
-  <si>
-    <t>SlowTurtleIdleSide.png</t>
-  </si>
-  <si>
-    <t>Basic Humanoid Sprites 1x.png</t>
-  </si>
-  <si>
-    <t>example_16x16.png</t>
-  </si>
-  <si>
-    <t>CuriousMonkeyIdleSide.png</t>
-  </si>
-  <si>
-    <t>Hearts5.png</t>
-  </si>
-  <si>
-    <t>Base.png</t>
-  </si>
-  <si>
-    <t>example_21x27.png</t>
-  </si>
-  <si>
-    <t>gothic-hero-crouch-slash_0006_Layer-7.png</t>
-  </si>
-  <si>
-    <t>Free Sprites 1x.png</t>
-  </si>
-  <si>
-    <t>01_dish.png</t>
-  </si>
-  <si>
-    <t>07_bread.png</t>
-  </si>
-  <si>
-    <t>35_donut_dish.png</t>
-  </si>
-  <si>
-    <t>34_donut.png</t>
-  </si>
-  <si>
-    <t>44_frenchfries.png</t>
-  </si>
-  <si>
-    <t>05_apple_pie.png</t>
-  </si>
-  <si>
-    <t>32_curry.png</t>
-  </si>
-  <si>
-    <t>24_cheesepuff.png</t>
-  </si>
-  <si>
-    <t>41_eggsalad_bowl.png</t>
-  </si>
-  <si>
-    <t>18_burrito.png</t>
-  </si>
-  <si>
-    <t>13_bacon.png</t>
-  </si>
-  <si>
-    <t>28_cookies.png</t>
-  </si>
-  <si>
-    <t>36_dumplings.png</t>
-  </si>
-  <si>
-    <t>11_bun.png</t>
-  </si>
-  <si>
-    <t>09_baguette.png</t>
-  </si>
-  <si>
-    <t>38_friedegg.png</t>
-  </si>
-  <si>
-    <t>15_burger.png</t>
-  </si>
-  <si>
-    <t>99_taco.png</t>
-  </si>
-  <si>
-    <t>22_cheesecake.png</t>
-  </si>
-  <si>
-    <t>30_chocolatecake.png</t>
-  </si>
-  <si>
-    <t>20_bagel.png</t>
-  </si>
-  <si>
-    <t>40_eggsalad.png</t>
-  </si>
-  <si>
-    <t>26_chocolate.png</t>
-  </si>
-  <si>
-    <t>42_eggtart.png</t>
-  </si>
-  <si>
-    <t>sprite_1.png</t>
-  </si>
-  <si>
-    <t>sprite_0.png</t>
-  </si>
-  <si>
-    <t>ghost-shriek.png</t>
-  </si>
-  <si>
-    <t>Wasp.png</t>
-  </si>
-  <si>
-    <t>hell-beast-breath.png</t>
-  </si>
-  <si>
-    <t>Scarab.png</t>
-  </si>
-  <si>
-    <t>wolf-runing-cycle.png</t>
-  </si>
-  <si>
-    <t>nightmare-idle.png</t>
-  </si>
-  <si>
-    <t>Assault-Class.png</t>
-  </si>
-  <si>
-    <t>Grenadier-Class.png</t>
-  </si>
-  <si>
-    <t>gothic-hero-crouch-slash_0002_Layer-3.png</t>
-  </si>
-  <si>
-    <t>example_128x128.png</t>
-  </si>
-  <si>
-    <t>demon-idle.png</t>
-  </si>
-  <si>
-    <t>town.png</t>
-  </si>
-  <si>
-    <t>clouds.png</t>
   </si>
   <si>
     <t>Subdivisão em grupos</t>
@@ -1444,13 +1513,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E52"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="43.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
@@ -1461,7 +1530,7 @@
     <col min="7" max="7" width="8.85714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1480,8 +1549,1005 @@
       <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1024</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>51.85546875</v>
+      </c>
+      <c r="E3">
+        <v>0.423007376957685</v>
+      </c>
+      <c r="F3">
+        <v>0.204164579510689</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1024</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>84.86328125</v>
+      </c>
+      <c r="E4">
+        <v>0.413880403570753</v>
+      </c>
+      <c r="F4">
+        <v>0.695303738117218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1024</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>60.15625</v>
+      </c>
+      <c r="E5">
+        <v>0.488426551688462</v>
+      </c>
+      <c r="F5">
+        <v>0.533390820026398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1024</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>96.6796875</v>
+      </c>
+      <c r="E6">
+        <v>0.410387155774515</v>
+      </c>
+      <c r="F6">
+        <v>0.606837868690491</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1024</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>96.484375</v>
+      </c>
+      <c r="E7">
+        <v>0.3291015625</v>
+      </c>
+      <c r="F7">
+        <v>0.623369753360748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>1024</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>94.04296875</v>
+      </c>
+      <c r="E8">
+        <v>0.32672945800914</v>
+      </c>
+      <c r="F8">
+        <v>0.709461510181427</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1024</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>97.75390625</v>
+      </c>
+      <c r="E9">
+        <v>0.3681640625</v>
+      </c>
+      <c r="F9">
+        <v>0.552709400653839</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>1024</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>93.45703125</v>
+      </c>
+      <c r="E10">
+        <v>0.393845290876925</v>
+      </c>
+      <c r="F10">
+        <v>0.709340214729309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1024</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>99.0234375</v>
+      </c>
+      <c r="E11">
+        <v>0.391262895686547</v>
+      </c>
+      <c r="F11">
+        <v>0.686295092105865</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>1024</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>98.828125</v>
+      </c>
+      <c r="E12">
+        <v>0.390354671282694</v>
+      </c>
+      <c r="F12">
+        <v>0.715250134468079</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>1024</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>90.625</v>
+      </c>
+      <c r="E13">
+        <v>0.417063148789263</v>
+      </c>
+      <c r="F13">
+        <v>0.665942907333374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>1024</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>99.90234375</v>
+      </c>
+      <c r="E14">
+        <v>0.354815455590142</v>
+      </c>
+      <c r="F14">
+        <v>0.647228419780731</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>1024</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>94.43359375</v>
+      </c>
+      <c r="E15">
+        <v>0.387622849385176</v>
+      </c>
+      <c r="F15">
+        <v>0.514358460903168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>1024</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>98.92578125</v>
+      </c>
+      <c r="E16">
+        <v>0.362630208333333</v>
+      </c>
+      <c r="F16">
+        <v>0.683717846870422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>1024</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>89.84375</v>
+      </c>
+      <c r="E17">
+        <v>0.388636957543592</v>
+      </c>
+      <c r="F17">
+        <v>0.706366300582886</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>1024</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>71.97265625</v>
+      </c>
+      <c r="E18">
+        <v>0.360404501872836</v>
+      </c>
+      <c r="F18">
+        <v>0.532127141952515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>1024</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>69.23828125</v>
+      </c>
+      <c r="E19">
+        <v>0.565699640729387</v>
+      </c>
+      <c r="F19">
+        <v>0.541957080364227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>1024</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>95.41015625</v>
+      </c>
+      <c r="E20">
+        <v>0.390014132193755</v>
+      </c>
+      <c r="F20">
+        <v>0.517609596252441</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>1024</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>97.55859375</v>
+      </c>
+      <c r="E21">
+        <v>0.355759353376925</v>
+      </c>
+      <c r="F21">
+        <v>0.602146625518799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>1024</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>99.31640625</v>
+      </c>
+      <c r="E22">
+        <v>0.402488941540166</v>
+      </c>
+      <c r="F22">
+        <v>0.720021605491638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>1024</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>91.30859375</v>
+      </c>
+      <c r="E23">
+        <v>0.551322282893428</v>
+      </c>
+      <c r="F23">
+        <v>0.386879593133926</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>1024</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="E24">
+        <v>0.375165576348081</v>
+      </c>
+      <c r="F24">
+        <v>0.634380877017975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>1024</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>82.91015625</v>
+      </c>
+      <c r="E25">
+        <v>0.357404979460019</v>
+      </c>
+      <c r="F25">
+        <v>0.660808861255646</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>1024</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>98.33984375</v>
+      </c>
+      <c r="E26">
+        <v>0.384473144338699</v>
+      </c>
+      <c r="F26">
+        <v>0.655570805072784</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>8960</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>92.9464285714286</v>
+      </c>
+      <c r="E27">
+        <v>0.370141068362275</v>
+      </c>
+      <c r="F27">
+        <v>0.566553950309753</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>360</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28">
+        <v>90.2777777777778</v>
+      </c>
+      <c r="E28">
+        <v>0.48328776686219</v>
+      </c>
+      <c r="F28">
+        <v>0.69773143529892</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>169</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>89.9408284023669</v>
+      </c>
+      <c r="E29">
+        <v>0.46786638757839</v>
+      </c>
+      <c r="F29">
+        <v>0.57273143529892</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>45056</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>70.8473899147727</v>
+      </c>
+      <c r="E30">
+        <v>0.322644179071975</v>
+      </c>
+      <c r="F30">
+        <v>0.804036259651184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>195</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31">
+        <v>92.3076923076923</v>
+      </c>
+      <c r="E31">
+        <v>0.498122286927114</v>
+      </c>
+      <c r="F31">
+        <v>0.659117519855499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>16616</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32">
+        <v>73.4954260953298</v>
+      </c>
+      <c r="E32">
+        <v>0.261009246696823</v>
+      </c>
+      <c r="F32">
+        <v>0.871571600437164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>13625</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>89.6880733944954</v>
+      </c>
+      <c r="E33">
+        <v>0.250411547016889</v>
+      </c>
+      <c r="F33">
+        <v>0.7022864818573</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>192</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34">
+        <v>88.5416666666667</v>
+      </c>
+      <c r="E34">
+        <v>0.468802923785511</v>
+      </c>
+      <c r="F34">
+        <v>0.571870505809784</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>567</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35">
+        <v>83.0687830687831</v>
+      </c>
+      <c r="E35">
+        <v>0.428648499843317</v>
+      </c>
+      <c r="F35">
+        <v>0.686707496643066</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36">
+        <v>960</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>80.7291666666667</v>
+      </c>
+      <c r="E36">
+        <v>0.50242454820416</v>
+      </c>
+      <c r="F36">
+        <v>0.511370658874512</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>1932</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>87.9399585921325</v>
+      </c>
+      <c r="E37">
+        <v>0.374669125774108</v>
+      </c>
+      <c r="F37">
+        <v>0.544112920761108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>10752</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38">
+        <v>94.3452380952381</v>
+      </c>
+      <c r="E38">
+        <v>0.340255519284371</v>
+      </c>
+      <c r="F38">
+        <v>0.410182029008865</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>957</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39">
+        <v>78.7878787878788</v>
+      </c>
+      <c r="E39">
+        <v>0.348686227386312</v>
+      </c>
+      <c r="F39">
+        <v>0.588086724281311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40">
+        <v>8960</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40">
+        <v>92.96875</v>
+      </c>
+      <c r="E40">
+        <v>0.363453409813727</v>
+      </c>
+      <c r="F40">
+        <v>0.58100038766861</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41">
+        <v>95.2380952380952</v>
+      </c>
+      <c r="E41">
+        <v>0.354497354497354</v>
+      </c>
+      <c r="F41">
+        <v>0.8255215883255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>342</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42">
+        <v>78.6549707602339</v>
+      </c>
+      <c r="E42">
+        <v>0.488304093567252</v>
+      </c>
+      <c r="F42">
+        <v>0.538527727127075</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43">
+        <v>2268</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43">
+        <v>67.636684303351</v>
+      </c>
+      <c r="E43">
+        <v>0.448141808249823</v>
+      </c>
+      <c r="F43">
+        <v>0.445090472698212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44">
+        <v>7371</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44">
+        <v>90.7610907610908</v>
+      </c>
+      <c r="E44">
+        <v>0.205904025252076</v>
+      </c>
+      <c r="F44">
+        <v>0.66362076997757</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45">
+        <v>6400</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45">
+        <v>62.1875</v>
+      </c>
+      <c r="E45">
+        <v>0.378343814107369</v>
+      </c>
+      <c r="F45">
+        <v>0.675796210765839</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46">
+        <v>144</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>96.5277777777778</v>
+      </c>
+      <c r="E46">
+        <v>0.535472467817642</v>
+      </c>
+      <c r="F46">
+        <v>0.689294040203094</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47">
+        <v>1485</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47">
+        <v>96.2962962962963</v>
+      </c>
+      <c r="E47">
+        <v>0.528264596536505</v>
+      </c>
+      <c r="F47">
+        <v>0.754867076873779</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48">
+        <v>1485</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48">
+        <v>92.6599326599327</v>
+      </c>
+      <c r="E48">
+        <v>0.36857903656601</v>
+      </c>
+      <c r="F48">
+        <v>0.646884024143219</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49">
+        <v>143</v>
+      </c>
+      <c r="C49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49">
+        <v>88.1118881118881</v>
+      </c>
+      <c r="E49">
+        <v>0.468017949021502</v>
+      </c>
+      <c r="F49">
+        <v>0.333616971969604</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50">
+        <v>45056</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50">
+        <v>62.2181285511364</v>
+      </c>
+      <c r="E50">
+        <v>0.488304259242134</v>
+      </c>
+      <c r="F50">
+        <v>0.602053344249725</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
+        <v>2048</v>
+      </c>
+      <c r="C51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51">
+        <v>97.900390625</v>
+      </c>
+      <c r="E51">
+        <v>0.382407202656926</v>
+      </c>
+      <c r="F51">
+        <v>0.616894960403442</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52">
+        <v>7168</v>
+      </c>
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52">
+        <v>45.1729910714286</v>
+      </c>
+      <c r="E52">
+        <v>0.380285999217969</v>
+      </c>
+      <c r="F52">
+        <v>0.497928887605667</v>
       </c>
     </row>
   </sheetData>
@@ -1526,12 +2592,12 @@
         <v>4</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:5">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B2" s="30">
         <v>63</v>
@@ -1548,7 +2614,7 @@
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B3" s="30">
         <v>143</v>
@@ -1565,7 +2631,7 @@
     </row>
     <row r="4" ht="18.75" customHeight="1" spans="1:5">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B4" s="30">
         <v>144</v>
@@ -1582,7 +2648,7 @@
     </row>
     <row r="5" ht="18.75" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B5" s="30">
         <v>169</v>
@@ -1599,7 +2665,7 @@
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B6" s="30">
         <v>192</v>
@@ -1616,7 +2682,7 @@
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:5">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B7" s="30">
         <v>195</v>
@@ -1633,7 +2699,7 @@
     </row>
     <row r="8" ht="18.75" customHeight="1" spans="1:5">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B8" s="30">
         <v>342</v>
@@ -1650,7 +2716,7 @@
     </row>
     <row r="9" ht="18.75" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B9" s="30">
         <v>360</v>
@@ -1667,7 +2733,7 @@
     </row>
     <row r="10" ht="18.75" customHeight="1" spans="1:5">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B10" s="30">
         <v>567</v>
@@ -1684,7 +2750,7 @@
     </row>
     <row r="11" ht="18.75" customHeight="1" spans="1:5">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B11" s="30">
         <v>957</v>
@@ -1701,7 +2767,7 @@
     </row>
     <row r="12" ht="18.75" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B12" s="30">
         <v>960</v>
@@ -1718,7 +2784,7 @@
     </row>
     <row r="13" ht="18.75" customHeight="1" spans="1:5">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B13" s="30">
         <v>1024</v>
@@ -1735,7 +2801,7 @@
     </row>
     <row r="14" ht="18.75" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B14" s="30">
         <v>1024</v>
@@ -1752,7 +2818,7 @@
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:5">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" s="30">
         <v>1024</v>
@@ -1786,7 +2852,7 @@
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:5">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B17" s="30">
         <v>1024</v>
@@ -1803,7 +2869,7 @@
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:5">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B18" s="30">
         <v>1024</v>
@@ -1820,7 +2886,7 @@
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:5">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" s="30">
         <v>1024</v>
@@ -1837,7 +2903,7 @@
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:5">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B20" s="30">
         <v>1024</v>
@@ -1871,7 +2937,7 @@
     </row>
     <row r="22" ht="18.75" customHeight="1" spans="1:5">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B22" s="30">
         <v>1024</v>
@@ -1888,7 +2954,7 @@
     </row>
     <row r="23" ht="18.75" customHeight="1" spans="1:5">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B23" s="30">
         <v>1024</v>
@@ -1905,7 +2971,7 @@
     </row>
     <row r="24" ht="18.75" customHeight="1" spans="1:8">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B24" s="30">
         <v>1024</v>
@@ -1926,7 +2992,7 @@
     </row>
     <row r="25" ht="18.75" customHeight="1" spans="1:8">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B25" s="30">
         <v>1024</v>
@@ -1947,7 +3013,7 @@
     </row>
     <row r="26" ht="18.75" customHeight="1" spans="1:8">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B26" s="30">
         <v>1024</v>
@@ -1968,7 +3034,7 @@
     </row>
     <row r="27" ht="18.75" customHeight="1" spans="1:5">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B27" s="30">
         <v>1024</v>
@@ -1985,7 +3051,7 @@
     </row>
     <row r="28" ht="18.75" customHeight="1" spans="1:5">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B28" s="30">
         <v>1024</v>
@@ -2002,7 +3068,7 @@
     </row>
     <row r="29" ht="18.75" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B29" s="30">
         <v>1024</v>
@@ -2019,7 +3085,7 @@
     </row>
     <row r="30" ht="18.75" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B30" s="30">
         <v>1024</v>
@@ -2036,7 +3102,7 @@
     </row>
     <row r="31" ht="18.75" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B31" s="30">
         <v>1024</v>
@@ -2053,7 +3119,7 @@
     </row>
     <row r="32" ht="18.75" customHeight="1" spans="1:5">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B32" s="30">
         <v>1024</v>
@@ -2070,7 +3136,7 @@
     </row>
     <row r="33" ht="18.75" customHeight="1" spans="1:5">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B33" s="30">
         <v>1024</v>
@@ -2087,7 +3153,7 @@
     </row>
     <row r="34" ht="18.75" customHeight="1" spans="1:5">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B34" s="30">
         <v>1024</v>
@@ -2104,7 +3170,7 @@
     </row>
     <row r="35" ht="18.75" customHeight="1" spans="1:5">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B35" s="30">
         <v>1024</v>
@@ -2121,7 +3187,7 @@
     </row>
     <row r="36" ht="18.75" customHeight="1" spans="1:5">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B36" s="30">
         <v>1024</v>
@@ -2138,7 +3204,7 @@
     </row>
     <row r="37" ht="18.75" customHeight="1" spans="1:5">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="B37" s="30">
         <v>1485</v>
@@ -2155,7 +3221,7 @@
     </row>
     <row r="38" ht="18.75" customHeight="1" spans="1:5">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B38" s="30">
         <v>1485</v>
@@ -2172,7 +3238,7 @@
     </row>
     <row r="39" ht="18.75" customHeight="1" spans="1:5">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B39" s="30">
         <v>1932</v>
@@ -2189,7 +3255,7 @@
     </row>
     <row r="40" ht="18.75" customHeight="1" spans="1:5">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B40" s="30">
         <v>2048</v>
@@ -2206,7 +3272,7 @@
     </row>
     <row r="41" ht="18.75" customHeight="1" spans="1:5">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B41" s="30">
         <v>2268</v>
@@ -2223,7 +3289,7 @@
     </row>
     <row r="42" ht="18.75" customHeight="1" spans="1:5">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B42" s="30">
         <v>6400</v>
@@ -2240,7 +3306,7 @@
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:5">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B43" s="30">
         <v>7168</v>
@@ -2257,7 +3323,7 @@
     </row>
     <row r="44" ht="18.75" customHeight="1" spans="1:5">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B44" s="30">
         <v>7371</v>
@@ -2274,7 +3340,7 @@
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:5">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B45" s="30">
         <v>8960</v>
@@ -2291,7 +3357,7 @@
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:5">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B46" s="30">
         <v>8960</v>
@@ -2325,7 +3391,7 @@
     </row>
     <row r="48" ht="18.75" customHeight="1" spans="1:5">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B48" s="30">
         <v>13625</v>
@@ -2342,7 +3408,7 @@
     </row>
     <row r="49" ht="18.75" customHeight="1" spans="1:5">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B49" s="30">
         <v>16616</v>
@@ -2359,7 +3425,7 @@
     </row>
     <row r="50" ht="18.75" customHeight="1" spans="1:5">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B50" s="30">
         <v>45056</v>
@@ -2376,7 +3442,7 @@
     </row>
     <row r="51" ht="18.75" customHeight="1" spans="1:5">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B51" s="30">
         <v>45056</v>
@@ -2419,39 +3485,39 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2504,7 +3570,7 @@
         <v>143</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H4" s="8">
         <f>MEDIAN(principal!E2:E12)</f>
@@ -2537,7 +3603,7 @@
         <v>144</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="H5" s="8">
         <f>MEDIAN(principal!C2:C12)</f>
@@ -2587,19 +3653,19 @@
         <v>192</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2652,7 +3718,7 @@
         <v>342</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H9" s="10">
         <f>MEDIAN(principal!E13:E41)</f>
@@ -2685,7 +3751,7 @@
         <v>360</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="H10" s="10">
         <f>MEDIAN(principal!C13:C41)</f>
@@ -2735,19 +3801,19 @@
         <v>957</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2800,7 +3866,7 @@
         <v>1024</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H14" s="13">
         <f>MEDIAN(principal!E42:E46)</f>
@@ -2833,7 +3899,7 @@
         <v>1024</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="H15" s="13">
         <f>MEDIAN(principal!C42:C46)</f>
@@ -2883,19 +3949,19 @@
         <v>1024</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2948,7 +4014,7 @@
         <v>1024</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H19" s="16">
         <f>MEDIAN(principal!E47:E51)</f>
@@ -2981,7 +4047,7 @@
         <v>1024</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="H20" s="16">
         <f>MEDIAN(principal!C47:C51)</f>
@@ -3371,7 +4437,7 @@
         <v>2268</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3446,16 +4512,16 @@
         <v>8960</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -3659,7 +4725,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B54">
         <v>1024</v>
@@ -3676,7 +4742,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B55">
         <v>1024</v>

</xml_diff>